<commit_message>
chart 5 progress re commit and push
</commit_message>
<xml_diff>
--- a/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
+++ b/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Research\EPISTAT\Lung Cancer\SOLC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex.Kim\code\lungcanceratlascharts\RE%3a_LC_Atlas_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="With ranks &amp; copy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="542">
   <si>
     <t>51 bar chart</t>
   </si>
@@ -1661,7 +1661,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1742,6 +1742,12 @@
     <font>
       <sz val="10"/>
       <color theme="0" tint="-0.499984740745262"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Lato"/>
       <family val="2"/>
     </font>
@@ -1952,7 +1958,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2179,6 +2185,8 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2464,10 +2472,10 @@
   <dimension ref="A1:AF58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="Q26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
+      <selection pane="bottomRight" activeCell="Q48" sqref="Q48:R54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2746,10 +2754,10 @@
       <c r="L4" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="96">
         <v>0.18840000000000001</v>
       </c>
-      <c r="N4" s="18">
+      <c r="N4" s="97">
         <v>0.4516</v>
       </c>
       <c r="O4" s="68" t="s">
@@ -2758,10 +2766,10 @@
       <c r="P4" s="19" t="s">
         <v>374</v>
       </c>
-      <c r="Q4" s="17">
+      <c r="Q4" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R4" s="18">
+      <c r="R4" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S4" s="68" t="s">
@@ -2844,10 +2852,10 @@
       <c r="P5" s="19" t="s">
         <v>377</v>
       </c>
-      <c r="Q5" s="17">
+      <c r="Q5" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R5" s="18">
+      <c r="R5" s="97">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="S5" s="68" t="s">
@@ -2930,10 +2938,10 @@
       <c r="P6" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="Q6" s="17">
+      <c r="Q6" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R6" s="18">
+      <c r="R6" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S6" s="68" t="s">
@@ -3016,10 +3024,10 @@
       <c r="P7" s="19" t="s">
         <v>385</v>
       </c>
-      <c r="Q7" s="17">
+      <c r="Q7" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R7" s="18">
+      <c r="R7" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S7" s="68" t="s">
@@ -3102,10 +3110,10 @@
       <c r="P8" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="Q8" s="96">
         <v>0.56899999999999995</v>
       </c>
-      <c r="R8" s="18">
+      <c r="R8" s="97">
         <v>0.05</v>
       </c>
       <c r="S8" s="68" t="s">
@@ -3188,10 +3196,10 @@
       <c r="P9" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="Q9" s="17">
+      <c r="Q9" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R9" s="18">
+      <c r="R9" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S9" s="68" t="s">
@@ -3274,10 +3282,10 @@
       <c r="P10" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="Q10" s="17">
+      <c r="Q10" s="96">
         <v>0.65300000000000002</v>
       </c>
-      <c r="R10" s="18">
+      <c r="R10" s="97">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="S10" s="68" t="s">
@@ -3360,10 +3368,10 @@
       <c r="P11" s="19" t="s">
         <v>399</v>
       </c>
-      <c r="Q11" s="17">
+      <c r="Q11" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R11" s="18">
+      <c r="R11" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S11" s="68" t="s">
@@ -3446,10 +3454,10 @@
       <c r="P12" s="19" t="s">
         <v>539</v>
       </c>
-      <c r="Q12" s="17">
+      <c r="Q12" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R12" s="18">
+      <c r="R12" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S12" s="68" t="s">
@@ -3532,10 +3540,10 @@
       <c r="P13" s="19" t="s">
         <v>402</v>
       </c>
-      <c r="Q13" s="17">
+      <c r="Q13" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R13" s="18">
+      <c r="R13" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S13" s="68" t="s">
@@ -3618,10 +3626,10 @@
       <c r="P14" s="19" t="s">
         <v>405</v>
       </c>
-      <c r="Q14" s="17">
+      <c r="Q14" s="96">
         <v>0.498</v>
       </c>
-      <c r="R14" s="18">
+      <c r="R14" s="97">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S14" s="68" t="s">
@@ -3704,10 +3712,10 @@
       <c r="P15" s="19" t="s">
         <v>408</v>
       </c>
-      <c r="Q15" s="17">
+      <c r="Q15" s="96">
         <v>0.59199999999999997</v>
       </c>
-      <c r="R15" s="18">
+      <c r="R15" s="97">
         <v>0.06</v>
       </c>
       <c r="S15" s="68" t="s">
@@ -3790,10 +3798,10 @@
       <c r="P16" s="19" t="s">
         <v>411</v>
       </c>
-      <c r="Q16" s="17">
+      <c r="Q16" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R16" s="18">
+      <c r="R16" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S16" s="68" t="s">
@@ -3876,10 +3884,10 @@
       <c r="P17" s="19" t="s">
         <v>414</v>
       </c>
-      <c r="Q17" s="17">
+      <c r="Q17" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R17" s="18">
+      <c r="R17" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S17" s="68" t="s">
@@ -3962,10 +3970,10 @@
       <c r="P18" s="19" t="s">
         <v>417</v>
       </c>
-      <c r="Q18" s="17">
+      <c r="Q18" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R18" s="18">
+      <c r="R18" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S18" s="68" t="s">
@@ -4048,10 +4056,10 @@
       <c r="P19" s="19" t="s">
         <v>420</v>
       </c>
-      <c r="Q19" s="17">
+      <c r="Q19" s="96">
         <v>0.499</v>
       </c>
-      <c r="R19" s="18">
+      <c r="R19" s="97">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="S19" s="68" t="s">
@@ -4134,10 +4142,10 @@
       <c r="P20" s="19" t="s">
         <v>423</v>
       </c>
-      <c r="Q20" s="17">
+      <c r="Q20" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R20" s="18">
+      <c r="R20" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S20" s="68" t="s">
@@ -4220,10 +4228,10 @@
       <c r="P21" s="19" t="s">
         <v>428</v>
       </c>
-      <c r="Q21" s="17">
+      <c r="Q21" s="96">
         <v>0.48799999999999999</v>
       </c>
-      <c r="R21" s="18">
+      <c r="R21" s="97">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="S21" s="68" t="s">
@@ -4306,10 +4314,10 @@
       <c r="P22" s="19" t="s">
         <v>432</v>
       </c>
-      <c r="Q22" s="17">
+      <c r="Q22" s="96">
         <v>0.41</v>
       </c>
-      <c r="R22" s="18">
+      <c r="R22" s="97">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="S22" s="68" t="s">
@@ -4392,10 +4400,10 @@
       <c r="P23" s="19" t="s">
         <v>435</v>
       </c>
-      <c r="Q23" s="17">
+      <c r="Q23" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R23" s="18">
+      <c r="R23" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S23" s="68" t="s">
@@ -4478,10 +4486,10 @@
       <c r="P24" s="19" t="s">
         <v>438</v>
       </c>
-      <c r="Q24" s="17">
+      <c r="Q24" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R24" s="18">
+      <c r="R24" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S24" s="68" t="s">
@@ -4564,10 +4572,10 @@
       <c r="P25" s="19" t="s">
         <v>441</v>
       </c>
-      <c r="Q25" s="17">
+      <c r="Q25" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R25" s="18">
+      <c r="R25" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S25" s="68" t="s">
@@ -4650,10 +4658,10 @@
       <c r="P26" s="19" t="s">
         <v>444</v>
       </c>
-      <c r="Q26" s="17">
+      <c r="Q26" s="96">
         <v>0.56299999999999994</v>
       </c>
-      <c r="R26" s="18">
+      <c r="R26" s="97">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="S26" s="68" t="s">
@@ -4736,10 +4744,10 @@
       <c r="P27" s="19" t="s">
         <v>447</v>
       </c>
-      <c r="Q27" s="17">
+      <c r="Q27" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R27" s="18">
+      <c r="R27" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S27" s="68" t="s">
@@ -4822,10 +4830,10 @@
       <c r="P28" s="19" t="s">
         <v>452</v>
       </c>
-      <c r="Q28" s="17">
+      <c r="Q28" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R28" s="18">
+      <c r="R28" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S28" s="68" t="s">
@@ -4908,10 +4916,10 @@
       <c r="P29" s="19" t="s">
         <v>455</v>
       </c>
-      <c r="Q29" s="17">
+      <c r="Q29" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R29" s="18">
+      <c r="R29" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S29" s="68" t="s">
@@ -4994,10 +5002,10 @@
       <c r="P30" s="19" t="s">
         <v>458</v>
       </c>
-      <c r="Q30" s="17">
+      <c r="Q30" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R30" s="18">
+      <c r="R30" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S30" s="68" t="s">
@@ -5080,10 +5088,10 @@
       <c r="P31" s="19" t="s">
         <v>461</v>
       </c>
-      <c r="Q31" s="17">
+      <c r="Q31" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R31" s="18">
+      <c r="R31" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S31" s="68" t="s">
@@ -5166,10 +5174,10 @@
       <c r="P32" s="19" t="s">
         <v>464</v>
       </c>
-      <c r="Q32" s="17">
+      <c r="Q32" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R32" s="18">
+      <c r="R32" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S32" s="68" t="s">
@@ -5252,10 +5260,10 @@
       <c r="P33" s="19" t="s">
         <v>467</v>
       </c>
-      <c r="Q33" s="17">
+      <c r="Q33" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R33" s="18">
+      <c r="R33" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S33" s="68" t="s">
@@ -5338,15 +5346,13 @@
       <c r="P34" s="19" t="s">
         <v>470</v>
       </c>
-      <c r="Q34" s="17">
+      <c r="Q34" s="96">
         <v>0.64700000000000002</v>
       </c>
-      <c r="R34" s="18">
+      <c r="R34" s="97">
         <v>4.7E-2</v>
       </c>
-      <c r="S34" s="68" t="s">
-        <v>68</v>
-      </c>
+      <c r="S34" s="68"/>
       <c r="T34" s="23">
         <v>0.25729999999999997</v>
       </c>
@@ -5424,10 +5430,10 @@
       <c r="P35" s="19" t="s">
         <v>473</v>
       </c>
-      <c r="Q35" s="17">
+      <c r="Q35" s="96">
         <v>0.48699999999999999</v>
       </c>
-      <c r="R35" s="18">
+      <c r="R35" s="97">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="S35" s="68" t="s">
@@ -5510,10 +5516,10 @@
       <c r="P36" s="19" t="s">
         <v>476</v>
       </c>
-      <c r="Q36" s="17">
+      <c r="Q36" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R36" s="18">
+      <c r="R36" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S36" s="68" t="s">
@@ -5596,10 +5602,10 @@
       <c r="P37" s="19" t="s">
         <v>479</v>
       </c>
-      <c r="Q37" s="17">
+      <c r="Q37" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R37" s="18">
+      <c r="R37" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S37" s="68" t="s">
@@ -5682,10 +5688,10 @@
       <c r="P38" s="19" t="s">
         <v>482</v>
       </c>
-      <c r="Q38" s="17">
+      <c r="Q38" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R38" s="18">
+      <c r="R38" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S38" s="68" t="s">
@@ -5768,10 +5774,10 @@
       <c r="P39" s="19" t="s">
         <v>485</v>
       </c>
-      <c r="Q39" s="17">
+      <c r="Q39" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R39" s="18">
+      <c r="R39" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S39" s="68" t="s">
@@ -5854,10 +5860,10 @@
       <c r="P40" s="19" t="s">
         <v>488</v>
       </c>
-      <c r="Q40" s="17">
+      <c r="Q40" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R40" s="18">
+      <c r="R40" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S40" s="68" t="s">
@@ -5940,10 +5946,10 @@
       <c r="P41" s="19" t="s">
         <v>491</v>
       </c>
-      <c r="Q41" s="17">
+      <c r="Q41" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R41" s="18">
+      <c r="R41" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S41" s="68" t="s">
@@ -6026,10 +6032,10 @@
       <c r="P42" s="19" t="s">
         <v>494</v>
       </c>
-      <c r="Q42" s="17">
+      <c r="Q42" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R42" s="18">
+      <c r="R42" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S42" s="68" t="s">
@@ -6112,10 +6118,10 @@
       <c r="P43" s="19" t="s">
         <v>497</v>
       </c>
-      <c r="Q43" s="17">
+      <c r="Q43" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R43" s="18">
+      <c r="R43" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S43" s="68" t="s">
@@ -6198,10 +6204,10 @@
       <c r="P44" s="19" t="s">
         <v>500</v>
       </c>
-      <c r="Q44" s="17">
+      <c r="Q44" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R44" s="18">
+      <c r="R44" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S44" s="68" t="s">
@@ -6284,10 +6290,10 @@
       <c r="P45" s="19" t="s">
         <v>503</v>
       </c>
-      <c r="Q45" s="17">
+      <c r="Q45" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R45" s="18">
+      <c r="R45" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S45" s="68" t="s">
@@ -6370,10 +6376,10 @@
       <c r="P46" s="19" t="s">
         <v>506</v>
       </c>
-      <c r="Q46" s="17">
+      <c r="Q46" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R46" s="18">
+      <c r="R46" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S46" s="68" t="s">
@@ -6456,10 +6462,10 @@
       <c r="P47" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="Q47" s="17">
+      <c r="Q47" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R47" s="18">
+      <c r="R47" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S47" s="68" t="s">
@@ -6542,10 +6548,10 @@
       <c r="P48" s="19" t="s">
         <v>514</v>
       </c>
-      <c r="Q48" s="17">
+      <c r="Q48" s="96">
         <v>0.56200000000000006</v>
       </c>
-      <c r="R48" s="18">
+      <c r="R48" s="97">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="S48" s="68" t="s">
@@ -6628,10 +6634,10 @@
       <c r="P49" s="19" t="s">
         <v>518</v>
       </c>
-      <c r="Q49" s="17">
+      <c r="Q49" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R49" s="18">
+      <c r="R49" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S49" s="68" t="s">
@@ -6714,10 +6720,10 @@
       <c r="P50" s="19" t="s">
         <v>521</v>
       </c>
-      <c r="Q50" s="17">
+      <c r="Q50" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R50" s="18">
+      <c r="R50" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S50" s="68" t="s">
@@ -6800,10 +6806,10 @@
       <c r="P51" s="19" t="s">
         <v>524</v>
       </c>
-      <c r="Q51" s="17">
+      <c r="Q51" s="96">
         <v>0.63600000000000001</v>
       </c>
-      <c r="R51" s="18">
+      <c r="R51" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S51" s="68" t="s">
@@ -6886,10 +6892,10 @@
       <c r="P52" s="19" t="s">
         <v>529</v>
       </c>
-      <c r="Q52" s="17">
+      <c r="Q52" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R52" s="18">
+      <c r="R52" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S52" s="68" t="s">
@@ -6972,10 +6978,10 @@
       <c r="P53" s="19" t="s">
         <v>532</v>
       </c>
-      <c r="Q53" s="17">
+      <c r="Q53" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R53" s="18">
+      <c r="R53" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S53" s="68" t="s">
@@ -7058,10 +7064,10 @@
       <c r="P54" s="19" t="s">
         <v>535</v>
       </c>
-      <c r="Q54" s="17">
+      <c r="Q54" s="96">
         <v>0.55300000000000005</v>
       </c>
-      <c r="R54" s="18">
+      <c r="R54" s="97">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="S54" s="68" t="s">

</xml_diff>

<commit_message>
making my way through states. finished up to DC
</commit_message>
<xml_diff>
--- a/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
+++ b/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="With ranks &amp; copy" sheetId="1" r:id="rId1"/>
@@ -2156,6 +2156,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2201,8 +2203,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2488,10 +2488,10 @@
   <dimension ref="A1:AF58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="U4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AF6" sqref="AF6"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2531,52 +2531,52 @@
   <sheetData>
     <row r="1" spans="1:32" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="97" t="s">
         <v>541</v>
       </c>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="93" t="s">
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="95" t="s">
         <v>544</v>
       </c>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="96" t="s">
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="98" t="s">
         <v>539</v>
       </c>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="98" t="s">
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="100" t="s">
         <v>539</v>
       </c>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="100" t="s">
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
+      <c r="O1" s="102" t="s">
         <v>542</v>
       </c>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="101" t="s">
+      <c r="P1" s="97"/>
+      <c r="Q1" s="97"/>
+      <c r="R1" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="102"/>
-      <c r="T1" s="102"/>
-      <c r="U1" s="91" t="s">
+      <c r="S1" s="104"/>
+      <c r="T1" s="104"/>
+      <c r="U1" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="V1" s="92"/>
-      <c r="W1" s="92"/>
-      <c r="X1" s="93" t="s">
+      <c r="V1" s="94"/>
+      <c r="W1" s="94"/>
+      <c r="X1" s="95" t="s">
         <v>543</v>
       </c>
-      <c r="Y1" s="94"/>
-      <c r="Z1" s="94"/>
-      <c r="AA1" s="88" t="s">
+      <c r="Y1" s="96"/>
+      <c r="Z1" s="96"/>
+      <c r="AA1" s="90" t="s">
         <v>540</v>
       </c>
-      <c r="AB1" s="89"/>
-      <c r="AC1" s="90"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="92"/>
       <c r="AD1" s="58" t="s">
         <v>123</v>
       </c>
@@ -2810,10 +2810,10 @@
       <c r="AC4" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="AD4" s="103" t="s">
+      <c r="AD4" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="AE4" s="104" t="s">
+      <c r="AE4" s="89" t="s">
         <v>74</v>
       </c>
       <c r="AF4" s="87" t="s">
@@ -2896,10 +2896,10 @@
       <c r="AC5" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="AD5" s="103" t="s">
+      <c r="AD5" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="AE5" s="104" t="s">
+      <c r="AE5" s="89" t="s">
         <v>76</v>
       </c>
       <c r="AF5" s="87" t="s">
@@ -2982,10 +2982,10 @@
       <c r="AC6" s="83" t="s">
         <v>129</v>
       </c>
-      <c r="AD6" s="103" t="s">
+      <c r="AD6" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="AE6" s="104" t="s">
+      <c r="AE6" s="89" t="s">
         <v>77</v>
       </c>
       <c r="AF6" s="87" t="s">
@@ -3002,7 +3002,7 @@
       <c r="C7" s="14">
         <v>49</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="83" t="s">
         <v>379</v>
       </c>
       <c r="E7" s="17" t="s">
@@ -3011,7 +3011,7 @@
       <c r="F7" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="83" t="s">
         <v>322</v>
       </c>
       <c r="H7" s="17">
@@ -3023,7 +3023,7 @@
       <c r="J7" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="84" t="s">
         <v>382</v>
       </c>
       <c r="L7" s="81">
@@ -3041,7 +3041,7 @@
       <c r="P7" s="24">
         <v>32</v>
       </c>
-      <c r="Q7" s="75" t="s">
+      <c r="Q7" s="85" t="s">
         <v>383</v>
       </c>
       <c r="R7" s="44"/>
@@ -3056,25 +3056,25 @@
       <c r="Y7" s="24">
         <v>38</v>
       </c>
-      <c r="Z7" s="76" t="s">
+      <c r="Z7" s="86" t="s">
         <v>174</v>
       </c>
       <c r="AA7" s="17">
         <v>0.24883340581347232</v>
       </c>
-      <c r="AB7" s="19" t="s">
+      <c r="AB7" s="84" t="s">
         <v>380</v>
       </c>
-      <c r="AC7" s="14" t="s">
+      <c r="AC7" s="83" t="s">
         <v>381</v>
       </c>
-      <c r="AD7" s="63" t="s">
+      <c r="AD7" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="AE7" s="64" t="s">
+      <c r="AE7" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="AF7" s="78" t="s">
+      <c r="AF7" s="87" t="s">
         <v>228</v>
       </c>
     </row>
@@ -3088,7 +3088,7 @@
       <c r="C8" s="14">
         <v>4</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="83" t="s">
         <v>384</v>
       </c>
       <c r="E8" s="17">
@@ -3097,7 +3097,7 @@
       <c r="F8" s="20">
         <v>10</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="83" t="s">
         <v>323</v>
       </c>
       <c r="H8" s="17">
@@ -3109,7 +3109,7 @@
       <c r="J8" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="84" t="s">
         <v>387</v>
       </c>
       <c r="L8" s="81">
@@ -3127,7 +3127,7 @@
       <c r="P8" s="24">
         <v>18</v>
       </c>
-      <c r="Q8" s="75" t="s">
+      <c r="Q8" s="85" t="s">
         <v>388</v>
       </c>
       <c r="R8" s="44"/>
@@ -3142,25 +3142,25 @@
       <c r="Y8" s="24">
         <v>45</v>
       </c>
-      <c r="Z8" s="76" t="s">
+      <c r="Z8" s="86" t="s">
         <v>175</v>
       </c>
       <c r="AA8" s="17">
         <v>0.11678356434966665</v>
       </c>
-      <c r="AB8" s="19" t="s">
+      <c r="AB8" s="84" t="s">
         <v>385</v>
       </c>
-      <c r="AC8" s="14" t="s">
+      <c r="AC8" s="83" t="s">
         <v>386</v>
       </c>
-      <c r="AD8" s="63" t="s">
+      <c r="AD8" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="AE8" s="64" t="s">
+      <c r="AE8" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="AF8" s="78" t="s">
+      <c r="AF8" s="87" t="s">
         <v>229</v>
       </c>
     </row>
@@ -3174,7 +3174,7 @@
       <c r="C9" s="14">
         <v>3</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="83" t="s">
         <v>389</v>
       </c>
       <c r="E9" s="17">
@@ -3183,7 +3183,7 @@
       <c r="F9" s="20">
         <v>6</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="83" t="s">
         <v>324</v>
       </c>
       <c r="H9" s="17">
@@ -3195,7 +3195,7 @@
       <c r="J9" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="84" t="s">
         <v>390</v>
       </c>
       <c r="L9" s="81">
@@ -3213,7 +3213,7 @@
       <c r="P9" s="24">
         <v>19</v>
       </c>
-      <c r="Q9" s="75" t="s">
+      <c r="Q9" s="85" t="s">
         <v>391</v>
       </c>
       <c r="R9" s="44"/>
@@ -3228,25 +3228,25 @@
       <c r="Y9" s="24">
         <v>15</v>
       </c>
-      <c r="Z9" s="76" t="s">
+      <c r="Z9" s="86" t="s">
         <v>205</v>
       </c>
       <c r="AA9" s="17">
         <v>0.15647582480563493</v>
       </c>
-      <c r="AB9" s="19" t="s">
+      <c r="AB9" s="84" t="s">
         <v>278</v>
       </c>
-      <c r="AC9" s="14" t="s">
+      <c r="AC9" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="AD9" s="63" t="s">
+      <c r="AD9" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="AE9" s="64" t="s">
+      <c r="AE9" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="AF9" s="78" t="s">
+      <c r="AF9" s="87" t="s">
         <v>230</v>
       </c>
     </row>
@@ -3326,10 +3326,10 @@
       <c r="AC10" s="83" t="s">
         <v>131</v>
       </c>
-      <c r="AD10" s="63" t="s">
+      <c r="AD10" s="88" t="s">
         <v>83</v>
       </c>
-      <c r="AE10" s="64" t="s">
+      <c r="AE10" s="89" t="s">
         <v>84</v>
       </c>
       <c r="AF10" s="87" t="s">
@@ -3346,7 +3346,7 @@
       <c r="C11" s="14">
         <v>42</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="83" t="s">
         <v>395</v>
       </c>
       <c r="E11" s="17" t="s">
@@ -3355,7 +3355,7 @@
       <c r="F11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="83" t="s">
         <v>326</v>
       </c>
       <c r="H11" s="17">
@@ -3367,7 +3367,7 @@
       <c r="J11" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="K11" s="84" t="s">
         <v>396</v>
       </c>
       <c r="L11" s="81">
@@ -3385,7 +3385,7 @@
       <c r="P11" s="24">
         <v>34</v>
       </c>
-      <c r="Q11" s="75" t="s">
+      <c r="Q11" s="85" t="s">
         <v>397</v>
       </c>
       <c r="R11" s="44"/>
@@ -3400,25 +3400,25 @@
       <c r="Y11" s="24">
         <v>1</v>
       </c>
-      <c r="Z11" s="76" t="s">
+      <c r="Z11" s="86" t="s">
         <v>177</v>
       </c>
       <c r="AA11" s="17">
         <v>0.17360395746617199</v>
       </c>
-      <c r="AB11" s="19" t="s">
+      <c r="AB11" s="84" t="s">
         <v>280</v>
       </c>
-      <c r="AC11" s="14" t="s">
+      <c r="AC11" s="83" t="s">
         <v>132</v>
       </c>
-      <c r="AD11" s="63" t="s">
+      <c r="AD11" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="AE11" s="64" t="s">
+      <c r="AE11" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="AF11" s="78" t="s">
+      <c r="AF11" s="87" t="s">
         <v>232</v>
       </c>
     </row>
@@ -3432,7 +3432,7 @@
       <c r="C12" s="14">
         <v>17</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="83" t="s">
         <v>534</v>
       </c>
       <c r="E12" s="17" t="s">
@@ -3441,7 +3441,7 @@
       <c r="F12" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="83" t="s">
         <v>327</v>
       </c>
       <c r="H12" s="17">
@@ -3453,7 +3453,7 @@
       <c r="J12" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="84" t="s">
         <v>536</v>
       </c>
       <c r="L12" s="81">
@@ -3471,7 +3471,7 @@
       <c r="P12" s="24">
         <v>30</v>
       </c>
-      <c r="Q12" s="75" t="s">
+      <c r="Q12" s="85" t="s">
         <v>537</v>
       </c>
       <c r="R12" s="44"/>
@@ -3486,25 +3486,25 @@
       <c r="Y12" s="24">
         <v>25</v>
       </c>
-      <c r="Z12" s="76" t="s">
+      <c r="Z12" s="86" t="s">
         <v>538</v>
       </c>
       <c r="AA12" s="17">
         <v>0.15994308319695427</v>
       </c>
-      <c r="AB12" s="19" t="s">
+      <c r="AB12" s="84" t="s">
         <v>535</v>
       </c>
-      <c r="AC12" s="14" t="s">
+      <c r="AC12" s="83" t="s">
         <v>273</v>
       </c>
-      <c r="AD12" s="63" t="s">
+      <c r="AD12" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="AE12" s="64" t="s">
+      <c r="AE12" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="AF12" s="78" t="s">
+      <c r="AF12" s="87" t="s">
         <v>274</v>
       </c>
     </row>

</xml_diff>

<commit_message>
did FL through IL
</commit_message>
<xml_diff>
--- a/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
+++ b/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
@@ -2488,10 +2488,10 @@
   <dimension ref="A1:AF58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="T4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="AF17" sqref="AF17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3518,7 +3518,7 @@
       <c r="C13" s="14">
         <v>26</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="83" t="s">
         <v>398</v>
       </c>
       <c r="E13" s="17" t="s">
@@ -3527,7 +3527,7 @@
       <c r="F13" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="83" t="s">
         <v>328</v>
       </c>
       <c r="H13" s="17">
@@ -3539,7 +3539,7 @@
       <c r="J13" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K13" s="19" t="s">
+      <c r="K13" s="84" t="s">
         <v>399</v>
       </c>
       <c r="L13" s="81">
@@ -3557,7 +3557,7 @@
       <c r="P13" s="24">
         <v>15</v>
       </c>
-      <c r="Q13" s="75" t="s">
+      <c r="Q13" s="85" t="s">
         <v>400</v>
       </c>
       <c r="R13" s="44"/>
@@ -3572,25 +3572,25 @@
       <c r="Y13" s="24">
         <v>21</v>
       </c>
-      <c r="Z13" s="76" t="s">
+      <c r="Z13" s="86" t="s">
         <v>206</v>
       </c>
       <c r="AA13" s="17">
         <v>0.15802004831552136</v>
       </c>
-      <c r="AB13" s="19" t="s">
+      <c r="AB13" s="84" t="s">
         <v>281</v>
       </c>
-      <c r="AC13" s="14" t="s">
+      <c r="AC13" s="83" t="s">
         <v>133</v>
       </c>
-      <c r="AD13" s="63" t="s">
+      <c r="AD13" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="AE13" s="64" t="s">
+      <c r="AE13" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="AF13" s="78" t="s">
+      <c r="AF13" s="87" t="s">
         <v>233</v>
       </c>
     </row>
@@ -3604,7 +3604,7 @@
       <c r="C14" s="14">
         <v>32</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="83" t="s">
         <v>401</v>
       </c>
       <c r="E14" s="17">
@@ -3613,7 +3613,7 @@
       <c r="F14" s="20">
         <v>23</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="83" t="s">
         <v>329</v>
       </c>
       <c r="H14" s="17">
@@ -3625,7 +3625,7 @@
       <c r="J14" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="84" t="s">
         <v>402</v>
       </c>
       <c r="L14" s="81">
@@ -3643,7 +3643,7 @@
       <c r="P14" s="24">
         <v>24</v>
       </c>
-      <c r="Q14" s="75" t="s">
+      <c r="Q14" s="85" t="s">
         <v>403</v>
       </c>
       <c r="R14" s="44"/>
@@ -3658,25 +3658,25 @@
       <c r="Y14" s="24">
         <v>31</v>
       </c>
-      <c r="Z14" s="76" t="s">
+      <c r="Z14" s="86" t="s">
         <v>178</v>
       </c>
       <c r="AA14" s="17">
         <v>0.17678297082342789</v>
       </c>
-      <c r="AB14" s="19" t="s">
+      <c r="AB14" s="84" t="s">
         <v>282</v>
       </c>
-      <c r="AC14" s="14" t="s">
+      <c r="AC14" s="83" t="s">
         <v>134</v>
       </c>
-      <c r="AD14" s="63" t="s">
+      <c r="AD14" s="88" t="s">
         <v>83</v>
       </c>
-      <c r="AE14" s="64" t="s">
+      <c r="AE14" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="AF14" s="78" t="s">
+      <c r="AF14" s="87" t="s">
         <v>234</v>
       </c>
     </row>
@@ -3690,7 +3690,7 @@
       <c r="C15" s="14">
         <v>5</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="83" t="s">
         <v>404</v>
       </c>
       <c r="E15" s="17">
@@ -3699,7 +3699,7 @@
       <c r="F15" s="20">
         <v>20</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="83" t="s">
         <v>330</v>
       </c>
       <c r="H15" s="17">
@@ -3711,7 +3711,7 @@
       <c r="J15" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K15" s="19" t="s">
+      <c r="K15" s="84" t="s">
         <v>405</v>
       </c>
       <c r="L15" s="81">
@@ -3729,7 +3729,7 @@
       <c r="P15" s="24">
         <v>39</v>
       </c>
-      <c r="Q15" s="75" t="s">
+      <c r="Q15" s="85" t="s">
         <v>406</v>
       </c>
       <c r="R15" s="44"/>
@@ -3744,25 +3744,25 @@
       <c r="Y15" s="24">
         <v>42</v>
       </c>
-      <c r="Z15" s="76" t="s">
+      <c r="Z15" s="86" t="s">
         <v>179</v>
       </c>
       <c r="AA15" s="17">
         <v>0.14093636018627745</v>
       </c>
-      <c r="AB15" s="19" t="s">
+      <c r="AB15" s="84" t="s">
         <v>283</v>
       </c>
-      <c r="AC15" s="14" t="s">
+      <c r="AC15" s="83" t="s">
         <v>135</v>
       </c>
-      <c r="AD15" s="63" t="s">
+      <c r="AD15" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="AE15" s="64" t="s">
+      <c r="AE15" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="AF15" s="78" t="s">
+      <c r="AF15" s="87" t="s">
         <v>235</v>
       </c>
     </row>
@@ -3776,7 +3776,7 @@
       <c r="C16" s="14">
         <v>7</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="83" t="s">
         <v>407</v>
       </c>
       <c r="E16" s="17">
@@ -3785,7 +3785,7 @@
       <c r="F16" s="20">
         <v>21</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="83" t="s">
         <v>331</v>
       </c>
       <c r="H16" s="17">
@@ -3797,7 +3797,7 @@
       <c r="J16" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="84" t="s">
         <v>408</v>
       </c>
       <c r="L16" s="81">
@@ -3815,7 +3815,7 @@
       <c r="P16" s="24">
         <v>29</v>
       </c>
-      <c r="Q16" s="75" t="s">
+      <c r="Q16" s="85" t="s">
         <v>409</v>
       </c>
       <c r="R16" s="44"/>
@@ -3830,25 +3830,25 @@
       <c r="Y16" s="24">
         <v>17</v>
       </c>
-      <c r="Z16" s="76" t="s">
+      <c r="Z16" s="86" t="s">
         <v>207</v>
       </c>
       <c r="AA16" s="17">
         <v>0.13843264085255502</v>
       </c>
-      <c r="AB16" s="19" t="s">
+      <c r="AB16" s="84" t="s">
         <v>284</v>
       </c>
-      <c r="AC16" s="14" t="s">
+      <c r="AC16" s="83" t="s">
         <v>136</v>
       </c>
-      <c r="AD16" s="63" t="s">
+      <c r="AD16" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="AE16" s="64" t="s">
+      <c r="AE16" s="89" t="s">
         <v>89</v>
       </c>
-      <c r="AF16" s="78" t="s">
+      <c r="AF16" s="87" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3862,7 +3862,7 @@
       <c r="C17" s="14">
         <v>35</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="83" t="s">
         <v>410</v>
       </c>
       <c r="E17" s="17">
@@ -3871,7 +3871,7 @@
       <c r="F17" s="20">
         <v>7</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="83" t="s">
         <v>332</v>
       </c>
       <c r="H17" s="17">
@@ -3883,7 +3883,7 @@
       <c r="J17" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K17" s="19" t="s">
+      <c r="K17" s="84" t="s">
         <v>411</v>
       </c>
       <c r="L17" s="81">
@@ -3901,7 +3901,7 @@
       <c r="P17" s="24">
         <v>10</v>
       </c>
-      <c r="Q17" s="75" t="s">
+      <c r="Q17" s="85" t="s">
         <v>412</v>
       </c>
       <c r="R17" s="44"/>
@@ -3916,25 +3916,25 @@
       <c r="Y17" s="24">
         <v>37</v>
       </c>
-      <c r="Z17" s="76" t="s">
+      <c r="Z17" s="86" t="s">
         <v>180</v>
       </c>
       <c r="AA17" s="17">
         <v>0.15129163664581946</v>
       </c>
-      <c r="AB17" s="19" t="s">
+      <c r="AB17" s="84" t="s">
         <v>285</v>
       </c>
-      <c r="AC17" s="14" t="s">
+      <c r="AC17" s="83" t="s">
         <v>137</v>
       </c>
-      <c r="AD17" s="63" t="s">
+      <c r="AD17" s="88" t="s">
         <v>90</v>
       </c>
-      <c r="AE17" s="64" t="s">
+      <c r="AE17" s="89" t="s">
         <v>91</v>
       </c>
-      <c r="AF17" s="78" t="s">
+      <c r="AF17" s="87" t="s">
         <v>237</v>
       </c>
     </row>

</xml_diff>

<commit_message>
did indiana throug louisiana
</commit_message>
<xml_diff>
--- a/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
+++ b/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
@@ -2487,11 +2487,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="T4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AF17" sqref="AF17"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3948,7 +3948,7 @@
       <c r="C18" s="14">
         <v>44</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="83" t="s">
         <v>413</v>
       </c>
       <c r="E18" s="17" t="s">
@@ -3957,7 +3957,7 @@
       <c r="F18" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="83" t="s">
         <v>333</v>
       </c>
       <c r="H18" s="17">
@@ -3969,7 +3969,7 @@
       <c r="J18" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K18" s="19" t="s">
+      <c r="K18" s="84" t="s">
         <v>414</v>
       </c>
       <c r="L18" s="81">
@@ -3987,7 +3987,7 @@
       <c r="P18" s="24">
         <v>42</v>
       </c>
-      <c r="Q18" s="75" t="s">
+      <c r="Q18" s="85" t="s">
         <v>415</v>
       </c>
       <c r="R18" s="44"/>
@@ -4002,25 +4002,25 @@
       <c r="Y18" s="24">
         <v>12</v>
       </c>
-      <c r="Z18" s="76" t="s">
+      <c r="Z18" s="86" t="s">
         <v>208</v>
       </c>
       <c r="AA18" s="17">
         <v>0.2055285375712991</v>
       </c>
-      <c r="AB18" s="19" t="s">
+      <c r="AB18" s="84" t="s">
         <v>286</v>
       </c>
-      <c r="AC18" s="14" t="s">
+      <c r="AC18" s="83" t="s">
         <v>138</v>
       </c>
-      <c r="AD18" s="63" t="s">
+      <c r="AD18" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="AE18" s="64" t="s">
+      <c r="AE18" s="89" t="s">
         <v>93</v>
       </c>
-      <c r="AF18" s="78" t="s">
+      <c r="AF18" s="87" t="s">
         <v>238</v>
       </c>
     </row>
@@ -4034,7 +4034,7 @@
       <c r="C19" s="14">
         <v>28</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="83" t="s">
         <v>416</v>
       </c>
       <c r="E19" s="17">
@@ -4043,7 +4043,7 @@
       <c r="F19" s="20">
         <v>25</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="83" t="s">
         <v>334</v>
       </c>
       <c r="H19" s="17">
@@ -4055,7 +4055,7 @@
       <c r="J19" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K19" s="19" t="s">
+      <c r="K19" s="84" t="s">
         <v>417</v>
       </c>
       <c r="L19" s="81">
@@ -4073,7 +4073,7 @@
       <c r="P19" s="24">
         <v>36</v>
       </c>
-      <c r="Q19" s="75" t="s">
+      <c r="Q19" s="85" t="s">
         <v>418</v>
       </c>
       <c r="R19" s="44"/>
@@ -4088,25 +4088,25 @@
       <c r="Y19" s="24">
         <v>24</v>
       </c>
-      <c r="Z19" s="76" t="s">
+      <c r="Z19" s="86" t="s">
         <v>209</v>
       </c>
       <c r="AA19" s="17">
         <v>0.18057406771974777</v>
       </c>
-      <c r="AB19" s="19" t="s">
+      <c r="AB19" s="84" t="s">
         <v>287</v>
       </c>
-      <c r="AC19" s="14" t="s">
+      <c r="AC19" s="83" t="s">
         <v>139</v>
       </c>
-      <c r="AD19" s="63" t="s">
+      <c r="AD19" s="88" t="s">
         <v>94</v>
       </c>
-      <c r="AE19" s="64" t="s">
+      <c r="AE19" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="AF19" s="78" t="s">
+      <c r="AF19" s="87" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4120,7 +4120,7 @@
       <c r="C20" s="14">
         <v>22</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="83" t="s">
         <v>419</v>
       </c>
       <c r="E20" s="17" t="s">
@@ -4129,7 +4129,7 @@
       <c r="F20" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="83" t="s">
         <v>335</v>
       </c>
       <c r="H20" s="17">
@@ -4141,7 +4141,7 @@
       <c r="J20" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="K20" s="19" t="s">
+      <c r="K20" s="84" t="s">
         <v>420</v>
       </c>
       <c r="L20" s="81">
@@ -4159,7 +4159,7 @@
       <c r="P20" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="Q20" s="75" t="s">
+      <c r="Q20" s="85" t="s">
         <v>421</v>
       </c>
       <c r="R20" s="44"/>
@@ -4174,25 +4174,25 @@
       <c r="Y20" s="24">
         <v>43</v>
       </c>
-      <c r="Z20" s="76" t="s">
+      <c r="Z20" s="86" t="s">
         <v>181</v>
       </c>
       <c r="AA20" s="17">
         <v>0.17715214387576331</v>
       </c>
-      <c r="AB20" s="19" t="s">
+      <c r="AB20" s="84" t="s">
         <v>288</v>
       </c>
-      <c r="AC20" s="14" t="s">
+      <c r="AC20" s="83" t="s">
         <v>140</v>
       </c>
-      <c r="AD20" s="63" t="s">
+      <c r="AD20" s="88" t="s">
         <v>95</v>
       </c>
-      <c r="AE20" s="64" t="s">
+      <c r="AE20" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="AF20" s="78" t="s">
+      <c r="AF20" s="87" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4206,7 +4206,7 @@
       <c r="C21" s="14">
         <v>51</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="83" t="s">
         <v>422</v>
       </c>
       <c r="E21" s="17">
@@ -4215,7 +4215,7 @@
       <c r="F21" s="20">
         <v>28</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="83" t="s">
         <v>336</v>
       </c>
       <c r="H21" s="17">
@@ -4227,7 +4227,7 @@
       <c r="J21" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K21" s="19" t="s">
+      <c r="K21" s="84" t="s">
         <v>425</v>
       </c>
       <c r="L21" s="81">
@@ -4245,7 +4245,7 @@
       <c r="P21" s="24">
         <v>12</v>
       </c>
-      <c r="Q21" s="75" t="s">
+      <c r="Q21" s="85" t="s">
         <v>426</v>
       </c>
       <c r="R21" s="44"/>
@@ -4260,25 +4260,25 @@
       <c r="Y21" s="24">
         <v>7</v>
       </c>
-      <c r="Z21" s="76" t="s">
+      <c r="Z21" s="86" t="s">
         <v>182</v>
       </c>
       <c r="AA21" s="17">
         <v>0.25946109971384973</v>
       </c>
-      <c r="AB21" s="19" t="s">
+      <c r="AB21" s="84" t="s">
         <v>423</v>
       </c>
-      <c r="AC21" s="14" t="s">
+      <c r="AC21" s="83" t="s">
         <v>424</v>
       </c>
-      <c r="AD21" s="63" t="s">
+      <c r="AD21" s="88" t="s">
         <v>97</v>
       </c>
-      <c r="AE21" s="64" t="s">
+      <c r="AE21" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="AF21" s="78" t="s">
+      <c r="AF21" s="87" t="s">
         <v>427</v>
       </c>
     </row>
@@ -4292,7 +4292,7 @@
       <c r="C22" s="14">
         <v>43</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="83" t="s">
         <v>428</v>
       </c>
       <c r="E22" s="17">
@@ -4301,7 +4301,7 @@
       <c r="F22" s="20">
         <v>31</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="83" t="s">
         <v>337</v>
       </c>
       <c r="H22" s="17">
@@ -4313,7 +4313,7 @@
       <c r="J22" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K22" s="19" t="s">
+      <c r="K22" s="84" t="s">
         <v>429</v>
       </c>
       <c r="L22" s="81">
@@ -4331,7 +4331,7 @@
       <c r="P22" s="24">
         <v>43</v>
       </c>
-      <c r="Q22" s="75" t="s">
+      <c r="Q22" s="85" t="s">
         <v>430</v>
       </c>
       <c r="R22" s="44"/>
@@ -4346,25 +4346,25 @@
       <c r="Y22" s="24">
         <v>35</v>
       </c>
-      <c r="Z22" s="76" t="s">
+      <c r="Z22" s="86" t="s">
         <v>183</v>
       </c>
       <c r="AA22" s="17">
         <v>0.21877266061966386</v>
       </c>
-      <c r="AB22" s="19" t="s">
+      <c r="AB22" s="84" t="s">
         <v>289</v>
       </c>
-      <c r="AC22" s="14" t="s">
+      <c r="AC22" s="83" t="s">
         <v>141</v>
       </c>
-      <c r="AD22" s="63" t="s">
+      <c r="AD22" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="AE22" s="64" t="s">
+      <c r="AE22" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="AF22" s="78" t="s">
+      <c r="AF22" s="87" t="s">
         <v>241</v>
       </c>
     </row>

</xml_diff>

<commit_message>
did maine through montana
</commit_message>
<xml_diff>
--- a/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
+++ b/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
@@ -2488,10 +2488,10 @@
   <dimension ref="A1:AF58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="R8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="AF30" sqref="AF30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4378,7 +4378,7 @@
       <c r="C23" s="14">
         <v>45</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="83" t="s">
         <v>431</v>
       </c>
       <c r="E23" s="17">
@@ -4387,7 +4387,7 @@
       <c r="F23" s="20">
         <v>10</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="83" t="s">
         <v>338</v>
       </c>
       <c r="H23" s="17">
@@ -4399,7 +4399,7 @@
       <c r="J23" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K23" s="19" t="s">
+      <c r="K23" s="84" t="s">
         <v>432</v>
       </c>
       <c r="L23" s="81">
@@ -4417,7 +4417,7 @@
       <c r="P23" s="24">
         <v>13</v>
       </c>
-      <c r="Q23" s="75" t="s">
+      <c r="Q23" s="85" t="s">
         <v>433</v>
       </c>
       <c r="R23" s="44"/>
@@ -4432,25 +4432,25 @@
       <c r="Y23" s="24">
         <v>23</v>
       </c>
-      <c r="Z23" s="76" t="s">
+      <c r="Z23" s="86" t="s">
         <v>210</v>
       </c>
       <c r="AA23" s="17">
         <v>0.19465813663811302</v>
       </c>
-      <c r="AB23" s="19" t="s">
+      <c r="AB23" s="84" t="s">
         <v>290</v>
       </c>
-      <c r="AC23" s="14" t="s">
+      <c r="AC23" s="83" t="s">
         <v>142</v>
       </c>
-      <c r="AD23" s="63" t="s">
+      <c r="AD23" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="AE23" s="64" t="s">
+      <c r="AE23" s="89" t="s">
         <v>83</v>
       </c>
-      <c r="AF23" s="78" t="s">
+      <c r="AF23" s="87" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4464,7 +4464,7 @@
       <c r="C24" s="14">
         <v>15</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="83" t="s">
         <v>434</v>
       </c>
       <c r="E24" s="17" t="s">
@@ -4473,7 +4473,7 @@
       <c r="F24" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="83" t="s">
         <v>339</v>
       </c>
       <c r="H24" s="17">
@@ -4485,7 +4485,7 @@
       <c r="J24" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K24" s="19" t="s">
+      <c r="K24" s="84" t="s">
         <v>435</v>
       </c>
       <c r="L24" s="81">
@@ -4503,7 +4503,7 @@
       <c r="P24" s="24">
         <v>8</v>
       </c>
-      <c r="Q24" s="75" t="s">
+      <c r="Q24" s="85" t="s">
         <v>436</v>
       </c>
       <c r="R24" s="44"/>
@@ -4518,25 +4518,25 @@
       <c r="Y24" s="24">
         <v>13</v>
       </c>
-      <c r="Z24" s="76" t="s">
+      <c r="Z24" s="86" t="s">
         <v>211</v>
       </c>
       <c r="AA24" s="17">
         <v>0.15117214410405386</v>
       </c>
-      <c r="AB24" s="19" t="s">
+      <c r="AB24" s="84" t="s">
         <v>291</v>
       </c>
-      <c r="AC24" s="14" t="s">
+      <c r="AC24" s="83" t="s">
         <v>143</v>
       </c>
-      <c r="AD24" s="63" t="s">
+      <c r="AD24" s="88" t="s">
         <v>99</v>
       </c>
-      <c r="AE24" s="64" t="s">
+      <c r="AE24" s="89" t="s">
         <v>99</v>
       </c>
-      <c r="AF24" s="78" t="s">
+      <c r="AF24" s="87" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4550,7 +4550,7 @@
       <c r="C25" s="14">
         <v>29</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="83" t="s">
         <v>437</v>
       </c>
       <c r="E25" s="17" t="s">
@@ -4559,7 +4559,7 @@
       <c r="F25" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="83" t="s">
         <v>340</v>
       </c>
       <c r="H25" s="17">
@@ -4571,7 +4571,7 @@
       <c r="J25" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K25" s="19" t="s">
+      <c r="K25" s="84" t="s">
         <v>438</v>
       </c>
       <c r="L25" s="81">
@@ -4589,7 +4589,7 @@
       <c r="P25" s="24">
         <v>1</v>
       </c>
-      <c r="Q25" s="75" t="s">
+      <c r="Q25" s="85" t="s">
         <v>439</v>
       </c>
       <c r="R25" s="44"/>
@@ -4604,25 +4604,25 @@
       <c r="Y25" s="24">
         <v>8</v>
       </c>
-      <c r="Z25" s="76" t="s">
+      <c r="Z25" s="86" t="s">
         <v>184</v>
       </c>
       <c r="AA25" s="17">
         <v>0.13991918454929686</v>
       </c>
-      <c r="AB25" s="19" t="s">
+      <c r="AB25" s="84" t="s">
         <v>292</v>
       </c>
-      <c r="AC25" s="14" t="s">
+      <c r="AC25" s="83" t="s">
         <v>144</v>
       </c>
-      <c r="AD25" s="63" t="s">
+      <c r="AD25" s="88" t="s">
         <v>84</v>
       </c>
-      <c r="AE25" s="64" t="s">
+      <c r="AE25" s="89" t="s">
         <v>100</v>
       </c>
-      <c r="AF25" s="78" t="s">
+      <c r="AF25" s="87" t="s">
         <v>244</v>
       </c>
     </row>
@@ -4636,7 +4636,7 @@
       <c r="C26" s="14">
         <v>33</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="83" t="s">
         <v>440</v>
       </c>
       <c r="E26" s="17" t="s">
@@ -4645,7 +4645,7 @@
       <c r="F26" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="83" t="s">
         <v>341</v>
       </c>
       <c r="H26" s="17">
@@ -4657,7 +4657,7 @@
       <c r="J26" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K26" s="19" t="s">
+      <c r="K26" s="84" t="s">
         <v>441</v>
       </c>
       <c r="L26" s="81">
@@ -4675,7 +4675,7 @@
       <c r="P26" s="24">
         <v>25</v>
       </c>
-      <c r="Q26" s="75" t="s">
+      <c r="Q26" s="85" t="s">
         <v>442</v>
       </c>
       <c r="R26" s="44"/>
@@ -4690,25 +4690,25 @@
       <c r="Y26" s="24">
         <v>18</v>
       </c>
-      <c r="Z26" s="76" t="s">
+      <c r="Z26" s="86" t="s">
         <v>212</v>
       </c>
       <c r="AA26" s="17">
         <v>0.20702453871969223</v>
       </c>
-      <c r="AB26" s="19" t="s">
+      <c r="AB26" s="84" t="s">
         <v>293</v>
       </c>
-      <c r="AC26" s="14" t="s">
+      <c r="AC26" s="83" t="s">
         <v>145</v>
       </c>
-      <c r="AD26" s="63" t="s">
+      <c r="AD26" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="AE26" s="64" t="s">
+      <c r="AE26" s="89" t="s">
         <v>101</v>
       </c>
-      <c r="AF26" s="78" t="s">
+      <c r="AF26" s="87" t="s">
         <v>245</v>
       </c>
     </row>
@@ -4722,7 +4722,7 @@
       <c r="C27" s="14">
         <v>9</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="83" t="s">
         <v>443</v>
       </c>
       <c r="E27" s="17" t="s">
@@ -4731,7 +4731,7 @@
       <c r="F27" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="83" t="s">
         <v>342</v>
       </c>
       <c r="H27" s="17">
@@ -4743,7 +4743,7 @@
       <c r="J27" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="K27" s="19" t="s">
+      <c r="K27" s="84" t="s">
         <v>444</v>
       </c>
       <c r="L27" s="81">
@@ -4761,7 +4761,7 @@
       <c r="P27" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="Q27" s="75" t="s">
+      <c r="Q27" s="85" t="s">
         <v>445</v>
       </c>
       <c r="R27" s="44"/>
@@ -4776,25 +4776,25 @@
       <c r="Y27" s="24">
         <v>34</v>
       </c>
-      <c r="Z27" s="76" t="s">
+      <c r="Z27" s="86" t="s">
         <v>185</v>
       </c>
       <c r="AA27" s="17">
         <v>0.16206774202352683</v>
       </c>
-      <c r="AB27" s="19" t="s">
+      <c r="AB27" s="84" t="s">
         <v>294</v>
       </c>
-      <c r="AC27" s="14" t="s">
+      <c r="AC27" s="83" t="s">
         <v>146</v>
       </c>
-      <c r="AD27" s="63" t="s">
+      <c r="AD27" s="88" t="s">
         <v>102</v>
       </c>
-      <c r="AE27" s="64" t="s">
+      <c r="AE27" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="AF27" s="78" t="s">
+      <c r="AF27" s="87" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4808,7 +4808,7 @@
       <c r="C28" s="14">
         <v>47</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="83" t="s">
         <v>446</v>
       </c>
       <c r="E28" s="17">
@@ -4817,7 +4817,7 @@
       <c r="F28" s="20">
         <v>28</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="83" t="s">
         <v>343</v>
       </c>
       <c r="H28" s="17">
@@ -4829,7 +4829,7 @@
       <c r="J28" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K28" s="19" t="s">
+      <c r="K28" s="84" t="s">
         <v>449</v>
       </c>
       <c r="L28" s="81">
@@ -4847,7 +4847,7 @@
       <c r="P28" s="24">
         <v>41</v>
       </c>
-      <c r="Q28" s="75" t="s">
+      <c r="Q28" s="85" t="s">
         <v>450</v>
       </c>
       <c r="R28" s="44"/>
@@ -4862,25 +4862,25 @@
       <c r="Y28" s="24">
         <v>29</v>
       </c>
-      <c r="Z28" s="76" t="s">
+      <c r="Z28" s="86" t="s">
         <v>213</v>
       </c>
       <c r="AA28" s="17">
         <v>0.22546283216479387</v>
       </c>
-      <c r="AB28" s="19" t="s">
+      <c r="AB28" s="84" t="s">
         <v>447</v>
       </c>
-      <c r="AC28" s="14" t="s">
+      <c r="AC28" s="83" t="s">
         <v>448</v>
       </c>
-      <c r="AD28" s="63" t="s">
+      <c r="AD28" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="AE28" s="64" t="s">
+      <c r="AE28" s="89" t="s">
         <v>99</v>
       </c>
-      <c r="AF28" s="78" t="s">
+      <c r="AF28" s="87" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4894,7 +4894,7 @@
       <c r="C29" s="14">
         <v>46</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="83" t="s">
         <v>451</v>
       </c>
       <c r="E29" s="17" t="s">
@@ -4903,7 +4903,7 @@
       <c r="F29" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="83" t="s">
         <v>344</v>
       </c>
       <c r="H29" s="17">
@@ -4915,7 +4915,7 @@
       <c r="J29" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K29" s="19" t="s">
+      <c r="K29" s="84" t="s">
         <v>452</v>
       </c>
       <c r="L29" s="81">
@@ -4933,7 +4933,7 @@
       <c r="P29" s="24">
         <v>27</v>
       </c>
-      <c r="Q29" s="75" t="s">
+      <c r="Q29" s="85" t="s">
         <v>453</v>
       </c>
       <c r="R29" s="44"/>
@@ -4948,25 +4948,25 @@
       <c r="Y29" s="24">
         <v>26</v>
       </c>
-      <c r="Z29" s="76" t="s">
+      <c r="Z29" s="86" t="s">
         <v>214</v>
       </c>
       <c r="AA29" s="17">
         <v>0.22256552446865413</v>
       </c>
-      <c r="AB29" s="19" t="s">
+      <c r="AB29" s="84" t="s">
         <v>295</v>
       </c>
-      <c r="AC29" s="14" t="s">
+      <c r="AC29" s="83" t="s">
         <v>147</v>
       </c>
-      <c r="AD29" s="63" t="s">
+      <c r="AD29" s="88" t="s">
         <v>103</v>
       </c>
-      <c r="AE29" s="64" t="s">
+      <c r="AE29" s="89" t="s">
         <v>104</v>
       </c>
-      <c r="AF29" s="78" t="s">
+      <c r="AF29" s="87" t="s">
         <v>248</v>
       </c>
     </row>
@@ -4980,7 +4980,7 @@
       <c r="C30" s="14">
         <v>13</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="83" t="s">
         <v>454</v>
       </c>
       <c r="E30" s="17">
@@ -4989,7 +4989,7 @@
       <c r="F30" s="20">
         <v>13</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="83" t="s">
         <v>345</v>
       </c>
       <c r="H30" s="17">
@@ -5001,7 +5001,7 @@
       <c r="J30" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K30" s="19" t="s">
+      <c r="K30" s="84" t="s">
         <v>455</v>
       </c>
       <c r="L30" s="81">
@@ -5019,7 +5019,7 @@
       <c r="P30" s="24">
         <v>31</v>
       </c>
-      <c r="Q30" s="75" t="s">
+      <c r="Q30" s="85" t="s">
         <v>456</v>
       </c>
       <c r="R30" s="44"/>
@@ -5034,25 +5034,25 @@
       <c r="Y30" s="24">
         <v>46</v>
       </c>
-      <c r="Z30" s="76" t="s">
+      <c r="Z30" s="86" t="s">
         <v>186</v>
       </c>
       <c r="AA30" s="17">
         <v>0.18910416661379192</v>
       </c>
-      <c r="AB30" s="19" t="s">
+      <c r="AB30" s="84" t="s">
         <v>296</v>
       </c>
-      <c r="AC30" s="14" t="s">
+      <c r="AC30" s="83" t="s">
         <v>148</v>
       </c>
-      <c r="AD30" s="63" t="s">
+      <c r="AD30" s="88" t="s">
         <v>105</v>
       </c>
-      <c r="AE30" s="64" t="s">
+      <c r="AE30" s="89" t="s">
         <v>106</v>
       </c>
-      <c r="AF30" s="78" t="s">
+      <c r="AF30" s="87" t="s">
         <v>249</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nebraska through north dakota
</commit_message>
<xml_diff>
--- a/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
+++ b/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
@@ -2488,10 +2488,10 @@
   <dimension ref="A1:AF58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="R8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="T18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AF30" sqref="AF30"/>
+      <selection pane="bottomRight" activeCell="AC40" sqref="AC40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5066,7 +5066,7 @@
       <c r="C31" s="14">
         <v>14</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="83" t="s">
         <v>457</v>
       </c>
       <c r="E31" s="17">
@@ -5075,7 +5075,7 @@
       <c r="F31" s="20">
         <v>15</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="83" t="s">
         <v>346</v>
       </c>
       <c r="H31" s="17">
@@ -5087,7 +5087,7 @@
       <c r="J31" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K31" s="19" t="s">
+      <c r="K31" s="84" t="s">
         <v>458</v>
       </c>
       <c r="L31" s="81">
@@ -5105,7 +5105,7 @@
       <c r="P31" s="24">
         <v>17</v>
       </c>
-      <c r="Q31" s="75" t="s">
+      <c r="Q31" s="85" t="s">
         <v>459</v>
       </c>
       <c r="R31" s="44"/>
@@ -5120,25 +5120,25 @@
       <c r="Y31" s="24">
         <v>40</v>
       </c>
-      <c r="Z31" s="76" t="s">
+      <c r="Z31" s="86" t="s">
         <v>187</v>
       </c>
       <c r="AA31" s="17">
         <v>0.17099298388282824</v>
       </c>
-      <c r="AB31" s="19" t="s">
+      <c r="AB31" s="84" t="s">
         <v>297</v>
       </c>
-      <c r="AC31" s="14" t="s">
+      <c r="AC31" s="83" t="s">
         <v>149</v>
       </c>
-      <c r="AD31" s="63" t="s">
+      <c r="AD31" s="88" t="s">
         <v>107</v>
       </c>
-      <c r="AE31" s="64" t="s">
+      <c r="AE31" s="89" t="s">
         <v>108</v>
       </c>
-      <c r="AF31" s="78" t="s">
+      <c r="AF31" s="87" t="s">
         <v>250</v>
       </c>
     </row>
@@ -5152,7 +5152,7 @@
       <c r="C32" s="14">
         <v>24</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="83" t="s">
         <v>460</v>
       </c>
       <c r="E32" s="17" t="s">
@@ -5161,7 +5161,7 @@
       <c r="F32" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="83" t="s">
         <v>347</v>
       </c>
       <c r="H32" s="17">
@@ -5173,7 +5173,7 @@
       <c r="J32" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K32" s="19" t="s">
+      <c r="K32" s="84" t="s">
         <v>461</v>
       </c>
       <c r="L32" s="81">
@@ -5191,7 +5191,7 @@
       <c r="P32" s="24">
         <v>37</v>
       </c>
-      <c r="Q32" s="75" t="s">
+      <c r="Q32" s="85" t="s">
         <v>462</v>
       </c>
       <c r="R32" s="44"/>
@@ -5206,25 +5206,25 @@
       <c r="Y32" s="24">
         <v>19</v>
       </c>
-      <c r="Z32" s="76" t="s">
+      <c r="Z32" s="86" t="s">
         <v>215</v>
       </c>
       <c r="AA32" s="17">
         <v>0.17547927543080832</v>
       </c>
-      <c r="AB32" s="19" t="s">
+      <c r="AB32" s="84" t="s">
         <v>298</v>
       </c>
-      <c r="AC32" s="14" t="s">
+      <c r="AC32" s="83" t="s">
         <v>150</v>
       </c>
-      <c r="AD32" s="63" t="s">
+      <c r="AD32" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="AE32" s="64" t="s">
+      <c r="AE32" s="89" t="s">
         <v>106</v>
       </c>
-      <c r="AF32" s="78" t="s">
+      <c r="AF32" s="87" t="s">
         <v>251</v>
       </c>
     </row>
@@ -5238,7 +5238,7 @@
       <c r="C33" s="14">
         <v>34</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="83" t="s">
         <v>463</v>
       </c>
       <c r="E33" s="17">
@@ -5247,7 +5247,7 @@
       <c r="F33" s="20">
         <v>3</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="83" t="s">
         <v>348</v>
       </c>
       <c r="H33" s="17">
@@ -5259,7 +5259,7 @@
       <c r="J33" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K33" s="19" t="s">
+      <c r="K33" s="84" t="s">
         <v>464</v>
       </c>
       <c r="L33" s="81">
@@ -5277,7 +5277,7 @@
       <c r="P33" s="24">
         <v>6</v>
       </c>
-      <c r="Q33" s="75" t="s">
+      <c r="Q33" s="85" t="s">
         <v>465</v>
       </c>
       <c r="R33" s="44"/>
@@ -5292,25 +5292,25 @@
       <c r="Y33" s="24">
         <v>5</v>
       </c>
-      <c r="Z33" s="76" t="s">
+      <c r="Z33" s="86" t="s">
         <v>188</v>
       </c>
       <c r="AA33" s="17">
         <v>0.15908732269244483</v>
       </c>
-      <c r="AB33" s="19" t="s">
+      <c r="AB33" s="84" t="s">
         <v>299</v>
       </c>
-      <c r="AC33" s="14" t="s">
+      <c r="AC33" s="83" t="s">
         <v>151</v>
       </c>
-      <c r="AD33" s="63" t="s">
+      <c r="AD33" s="88" t="s">
         <v>85</v>
       </c>
-      <c r="AE33" s="64" t="s">
+      <c r="AE33" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="AF33" s="78" t="s">
+      <c r="AF33" s="87" t="s">
         <v>252</v>
       </c>
     </row>
@@ -5324,7 +5324,7 @@
       <c r="C34" s="14">
         <v>16</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="83" t="s">
         <v>466</v>
       </c>
       <c r="E34" s="17">
@@ -5333,7 +5333,7 @@
       <c r="F34" s="20">
         <v>4</v>
       </c>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="83" t="s">
         <v>349</v>
       </c>
       <c r="H34" s="17">
@@ -5345,7 +5345,7 @@
       <c r="J34" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K34" s="19" t="s">
+      <c r="K34" s="84" t="s">
         <v>467</v>
       </c>
       <c r="L34" s="81">
@@ -5361,7 +5361,7 @@
       <c r="P34" s="24">
         <v>4</v>
       </c>
-      <c r="Q34" s="75" t="s">
+      <c r="Q34" s="85" t="s">
         <v>468</v>
       </c>
       <c r="R34" s="44"/>
@@ -5376,22 +5376,22 @@
       <c r="Y34" s="24">
         <v>4</v>
       </c>
-      <c r="Z34" s="76" t="s">
+      <c r="Z34" s="86" t="s">
         <v>189</v>
       </c>
       <c r="AA34" s="17">
         <v>0.13529447263799368</v>
       </c>
-      <c r="AB34" s="19" t="s">
+      <c r="AB34" s="84" t="s">
         <v>300</v>
       </c>
-      <c r="AC34" s="14" t="s">
+      <c r="AC34" s="83" t="s">
         <v>152</v>
       </c>
-      <c r="AD34" s="63" t="s">
+      <c r="AD34" s="88" t="s">
         <v>106</v>
       </c>
-      <c r="AE34" s="64" t="s">
+      <c r="AE34" s="89" t="s">
         <v>103</v>
       </c>
       <c r="AF34" s="78" t="s">
@@ -5408,7 +5408,7 @@
       <c r="C35" s="14">
         <v>2</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="83" t="s">
         <v>469</v>
       </c>
       <c r="E35" s="17">
@@ -5417,7 +5417,7 @@
       <c r="F35" s="20">
         <v>26</v>
       </c>
-      <c r="G35" s="14" t="s">
+      <c r="G35" s="83" t="s">
         <v>350</v>
       </c>
       <c r="H35" s="17">
@@ -5429,7 +5429,7 @@
       <c r="J35" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K35" s="19" t="s">
+      <c r="K35" s="84" t="s">
         <v>470</v>
       </c>
       <c r="L35" s="81">
@@ -5447,7 +5447,7 @@
       <c r="P35" s="24">
         <v>46</v>
       </c>
-      <c r="Q35" s="75" t="s">
+      <c r="Q35" s="85" t="s">
         <v>471</v>
       </c>
       <c r="R35" s="44"/>
@@ -5462,22 +5462,22 @@
       <c r="Y35" s="24">
         <v>47</v>
       </c>
-      <c r="Z35" s="76" t="s">
+      <c r="Z35" s="86" t="s">
         <v>190</v>
       </c>
       <c r="AA35" s="17">
         <v>0.1752603184894628</v>
       </c>
-      <c r="AB35" s="19" t="s">
+      <c r="AB35" s="84" t="s">
         <v>301</v>
       </c>
-      <c r="AC35" s="14" t="s">
+      <c r="AC35" s="83" t="s">
         <v>153</v>
       </c>
-      <c r="AD35" s="63" t="s">
+      <c r="AD35" s="88" t="s">
         <v>106</v>
       </c>
-      <c r="AE35" s="64" t="s">
+      <c r="AE35" s="89" t="s">
         <v>109</v>
       </c>
       <c r="AF35" s="78" t="s">
@@ -5494,7 +5494,7 @@
       <c r="C36" s="14">
         <v>21</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="83" t="s">
         <v>472</v>
       </c>
       <c r="E36" s="17">
@@ -5503,7 +5503,7 @@
       <c r="F36" s="20">
         <v>1</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="G36" s="83" t="s">
         <v>351</v>
       </c>
       <c r="H36" s="17">
@@ -5515,7 +5515,7 @@
       <c r="J36" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K36" s="19" t="s">
+      <c r="K36" s="84" t="s">
         <v>473</v>
       </c>
       <c r="L36" s="81">
@@ -5533,7 +5533,7 @@
       <c r="P36" s="24">
         <v>3</v>
       </c>
-      <c r="Q36" s="75" t="s">
+      <c r="Q36" s="85" t="s">
         <v>474</v>
       </c>
       <c r="R36" s="44"/>
@@ -5548,22 +5548,22 @@
       <c r="Y36" s="24">
         <v>10</v>
       </c>
-      <c r="Z36" s="76" t="s">
+      <c r="Z36" s="86" t="s">
         <v>216</v>
       </c>
       <c r="AA36" s="17">
         <v>0.15219249928945883</v>
       </c>
-      <c r="AB36" s="19" t="s">
+      <c r="AB36" s="84" t="s">
         <v>302</v>
       </c>
-      <c r="AC36" s="14" t="s">
+      <c r="AC36" s="83" t="s">
         <v>154</v>
       </c>
-      <c r="AD36" s="63" t="s">
+      <c r="AD36" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="AE36" s="64" t="s">
+      <c r="AE36" s="89" t="s">
         <v>73</v>
       </c>
       <c r="AF36" s="78" t="s">
@@ -5580,7 +5580,7 @@
       <c r="C37" s="14">
         <v>38</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="83" t="s">
         <v>475</v>
       </c>
       <c r="E37" s="17">
@@ -5589,7 +5589,7 @@
       <c r="F37" s="20">
         <v>17</v>
       </c>
-      <c r="G37" s="14" t="s">
+      <c r="G37" s="83" t="s">
         <v>352</v>
       </c>
       <c r="H37" s="17">
@@ -5601,7 +5601,7 @@
       <c r="J37" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K37" s="19" t="s">
+      <c r="K37" s="84" t="s">
         <v>476</v>
       </c>
       <c r="L37" s="81">
@@ -5619,7 +5619,7 @@
       <c r="P37" s="24">
         <v>21</v>
       </c>
-      <c r="Q37" s="75" t="s">
+      <c r="Q37" s="85" t="s">
         <v>477</v>
       </c>
       <c r="R37" s="44"/>
@@ -5634,25 +5634,25 @@
       <c r="Y37" s="24">
         <v>14</v>
       </c>
-      <c r="Z37" s="76" t="s">
+      <c r="Z37" s="86" t="s">
         <v>217</v>
       </c>
       <c r="AA37" s="17">
         <v>0.18993389204543945</v>
       </c>
-      <c r="AB37" s="19" t="s">
+      <c r="AB37" s="84" t="s">
         <v>303</v>
       </c>
-      <c r="AC37" s="14" t="s">
+      <c r="AC37" s="83" t="s">
         <v>155</v>
       </c>
-      <c r="AD37" s="63" t="s">
+      <c r="AD37" s="88" t="s">
         <v>99</v>
       </c>
-      <c r="AE37" s="64" t="s">
+      <c r="AE37" s="89" t="s">
         <v>111</v>
       </c>
-      <c r="AF37" s="78" t="s">
+      <c r="AF37" s="87" t="s">
         <v>256</v>
       </c>
     </row>
@@ -5666,7 +5666,7 @@
       <c r="C38" s="14">
         <v>11</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="83" t="s">
         <v>478</v>
       </c>
       <c r="E38" s="17">
@@ -5675,7 +5675,7 @@
       <c r="F38" s="20">
         <v>8</v>
       </c>
-      <c r="G38" s="14" t="s">
+      <c r="G38" s="83" t="s">
         <v>353</v>
       </c>
       <c r="H38" s="17">
@@ -5687,7 +5687,7 @@
       <c r="J38" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K38" s="19" t="s">
+      <c r="K38" s="84" t="s">
         <v>479</v>
       </c>
       <c r="L38" s="81">
@@ -5705,7 +5705,7 @@
       <c r="P38" s="24">
         <v>14</v>
       </c>
-      <c r="Q38" s="75" t="s">
+      <c r="Q38" s="85" t="s">
         <v>480</v>
       </c>
       <c r="R38" s="44"/>
@@ -5720,25 +5720,25 @@
       <c r="Y38" s="24">
         <v>44</v>
       </c>
-      <c r="Z38" s="76" t="s">
+      <c r="Z38" s="86" t="s">
         <v>191</v>
       </c>
       <c r="AA38" s="17">
         <v>0.18714265521749884</v>
       </c>
-      <c r="AB38" s="19" t="s">
+      <c r="AB38" s="84" t="s">
         <v>304</v>
       </c>
-      <c r="AC38" s="14" t="s">
+      <c r="AC38" s="83" t="s">
         <v>156</v>
       </c>
-      <c r="AD38" s="63" t="s">
+      <c r="AD38" s="88" t="s">
         <v>107</v>
       </c>
-      <c r="AE38" s="64" t="s">
+      <c r="AE38" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="AF38" s="78" t="s">
+      <c r="AF38" s="87" t="s">
         <v>257</v>
       </c>
     </row>

</xml_diff>

<commit_message>
did ohio through south dakota
</commit_message>
<xml_diff>
--- a/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
+++ b/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
@@ -1670,7 +1670,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1759,6 +1759,14 @@
       <sz val="10"/>
       <name val="Lato"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1967,7 +1975,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2203,6 +2211,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2488,10 +2497,10 @@
   <dimension ref="A1:AF58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="T18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="O26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AC40" sqref="AC40"/>
+      <selection pane="bottomRight" activeCell="AF45" sqref="AF45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2513,11 +2522,11 @@
     <col min="16" max="16" width="5.140625" style="29" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="24.28515625" style="26" customWidth="1"/>
     <col min="18" max="18" width="10.7109375" style="34" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="34" customWidth="1"/>
-    <col min="20" max="20" width="41.85546875" style="52" customWidth="1"/>
-    <col min="21" max="21" width="7.5703125" style="34" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.85546875" style="34" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" style="34" customWidth="1"/>
+    <col min="20" max="20" width="41.85546875" style="52" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5703125" style="34" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="5.140625" style="50" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" style="34" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="10.85546875" style="26" customWidth="1"/>
     <col min="25" max="25" width="5.140625" style="29" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="48.5703125" style="26" customWidth="1"/>
@@ -5394,7 +5403,7 @@
       <c r="AE34" s="89" t="s">
         <v>103</v>
       </c>
-      <c r="AF34" s="78" t="s">
+      <c r="AF34" s="87" t="s">
         <v>253</v>
       </c>
     </row>
@@ -5480,7 +5489,7 @@
       <c r="AE35" s="89" t="s">
         <v>109</v>
       </c>
-      <c r="AF35" s="78" t="s">
+      <c r="AF35" s="87" t="s">
         <v>254</v>
       </c>
     </row>
@@ -5566,7 +5575,7 @@
       <c r="AE36" s="89" t="s">
         <v>73</v>
       </c>
-      <c r="AF36" s="78" t="s">
+      <c r="AF36" s="87" t="s">
         <v>255</v>
       </c>
     </row>
@@ -5752,7 +5761,7 @@
       <c r="C39" s="14">
         <v>39</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D39" s="83" t="s">
         <v>481</v>
       </c>
       <c r="E39" s="17" t="s">
@@ -5761,7 +5770,7 @@
       <c r="F39" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G39" s="14" t="s">
+      <c r="G39" s="83" t="s">
         <v>354</v>
       </c>
       <c r="H39" s="17">
@@ -5773,7 +5782,7 @@
       <c r="J39" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K39" s="19" t="s">
+      <c r="K39" s="84" t="s">
         <v>482</v>
       </c>
       <c r="L39" s="81">
@@ -5791,7 +5800,7 @@
       <c r="P39" s="24">
         <v>22</v>
       </c>
-      <c r="Q39" s="75" t="s">
+      <c r="Q39" s="85" t="s">
         <v>483</v>
       </c>
       <c r="R39" s="44"/>
@@ -5806,29 +5815,29 @@
       <c r="Y39" s="24">
         <v>36</v>
       </c>
-      <c r="Z39" s="76" t="s">
+      <c r="Z39" s="86" t="s">
         <v>192</v>
       </c>
       <c r="AA39" s="17">
         <v>0.21561882598347776</v>
       </c>
-      <c r="AB39" s="19" t="s">
+      <c r="AB39" s="84" t="s">
         <v>305</v>
       </c>
-      <c r="AC39" s="14" t="s">
+      <c r="AC39" s="83" t="s">
         <v>157</v>
       </c>
-      <c r="AD39" s="63" t="s">
+      <c r="AD39" s="88" t="s">
         <v>107</v>
       </c>
-      <c r="AE39" s="64" t="s">
+      <c r="AE39" s="89" t="s">
         <v>93</v>
       </c>
-      <c r="AF39" s="78" t="s">
+      <c r="AF39" s="87" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="40" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>53</v>
       </c>
@@ -5838,7 +5847,7 @@
       <c r="C40" s="14">
         <v>40</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="83" t="s">
         <v>484</v>
       </c>
       <c r="E40" s="17" t="s">
@@ -5847,7 +5856,7 @@
       <c r="F40" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="G40" s="83" t="s">
         <v>355</v>
       </c>
       <c r="H40" s="17">
@@ -5859,7 +5868,7 @@
       <c r="J40" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K40" s="19" t="s">
+      <c r="K40" s="84" t="s">
         <v>485</v>
       </c>
       <c r="L40" s="81">
@@ -5877,7 +5886,7 @@
       <c r="P40" s="24">
         <v>48</v>
       </c>
-      <c r="Q40" s="75" t="s">
+      <c r="Q40" s="85" t="s">
         <v>486</v>
       </c>
       <c r="R40" s="44"/>
@@ -5892,25 +5901,25 @@
       <c r="Y40" s="24">
         <v>48</v>
       </c>
-      <c r="Z40" s="76" t="s">
+      <c r="Z40" s="86" t="s">
         <v>193</v>
       </c>
       <c r="AA40" s="17">
         <v>0.22154467361085187</v>
       </c>
-      <c r="AB40" s="19" t="s">
+      <c r="AB40" s="105" t="s">
         <v>306</v>
       </c>
-      <c r="AC40" s="14" t="s">
+      <c r="AC40" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="AD40" s="63" t="s">
+      <c r="AD40" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="AE40" s="64" t="s">
+      <c r="AE40" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="AF40" s="78" t="s">
+      <c r="AF40" s="87" t="s">
         <v>259</v>
       </c>
     </row>
@@ -5924,7 +5933,7 @@
       <c r="C41" s="14">
         <v>18</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41" s="83" t="s">
         <v>487</v>
       </c>
       <c r="E41" s="17" t="s">
@@ -5933,7 +5942,7 @@
       <c r="F41" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G41" s="14" t="s">
+      <c r="G41" s="83" t="s">
         <v>356</v>
       </c>
       <c r="H41" s="17">
@@ -5945,7 +5954,7 @@
       <c r="J41" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K41" s="19" t="s">
+      <c r="K41" s="84" t="s">
         <v>488</v>
       </c>
       <c r="L41" s="81">
@@ -5963,7 +5972,7 @@
       <c r="P41" s="24">
         <v>28</v>
       </c>
-      <c r="Q41" s="75" t="s">
+      <c r="Q41" s="85" t="s">
         <v>489</v>
       </c>
       <c r="R41" s="44"/>
@@ -5978,25 +5987,25 @@
       <c r="Y41" s="24">
         <v>33</v>
       </c>
-      <c r="Z41" s="76" t="s">
+      <c r="Z41" s="86" t="s">
         <v>194</v>
       </c>
       <c r="AA41" s="17">
         <v>0.17118381997147342</v>
       </c>
-      <c r="AB41" s="19" t="s">
+      <c r="AB41" s="84" t="s">
         <v>307</v>
       </c>
-      <c r="AC41" s="14" t="s">
+      <c r="AC41" s="83" t="s">
         <v>159</v>
       </c>
-      <c r="AD41" s="63" t="s">
+      <c r="AD41" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="AE41" s="64" t="s">
+      <c r="AE41" s="89" t="s">
         <v>112</v>
       </c>
-      <c r="AF41" s="78" t="s">
+      <c r="AF41" s="87" t="s">
         <v>260</v>
       </c>
     </row>
@@ -6010,7 +6019,7 @@
       <c r="C42" s="14">
         <v>30</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="83" t="s">
         <v>490</v>
       </c>
       <c r="E42" s="17">
@@ -6019,7 +6028,7 @@
       <c r="F42" s="20">
         <v>9</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="83" t="s">
         <v>357</v>
       </c>
       <c r="H42" s="17">
@@ -6031,7 +6040,7 @@
       <c r="J42" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K42" s="19" t="s">
+      <c r="K42" s="84" t="s">
         <v>491</v>
       </c>
       <c r="L42" s="81">
@@ -6049,7 +6058,7 @@
       <c r="P42" s="24">
         <v>11</v>
       </c>
-      <c r="Q42" s="75" t="s">
+      <c r="Q42" s="85" t="s">
         <v>492</v>
       </c>
       <c r="R42" s="44"/>
@@ -6064,25 +6073,25 @@
       <c r="Y42" s="24">
         <v>6</v>
       </c>
-      <c r="Z42" s="76" t="s">
+      <c r="Z42" s="86" t="s">
         <v>195</v>
       </c>
       <c r="AA42" s="17">
         <v>0.18127382464402422</v>
       </c>
-      <c r="AB42" s="19" t="s">
+      <c r="AB42" s="84" t="s">
         <v>308</v>
       </c>
-      <c r="AC42" s="14" t="s">
+      <c r="AC42" s="83" t="s">
         <v>160</v>
       </c>
-      <c r="AD42" s="63" t="s">
+      <c r="AD42" s="88" t="s">
         <v>113</v>
       </c>
-      <c r="AE42" s="64" t="s">
+      <c r="AE42" s="89" t="s">
         <v>114</v>
       </c>
-      <c r="AF42" s="78" t="s">
+      <c r="AF42" s="87" t="s">
         <v>261</v>
       </c>
     </row>
@@ -6096,7 +6105,7 @@
       <c r="C43" s="14">
         <v>37</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D43" s="83" t="s">
         <v>493</v>
       </c>
       <c r="E43" s="17">
@@ -6105,7 +6114,7 @@
       <c r="F43" s="20">
         <v>5</v>
       </c>
-      <c r="G43" s="14" t="s">
+      <c r="G43" s="83" t="s">
         <v>358</v>
       </c>
       <c r="H43" s="17">
@@ -6117,7 +6126,7 @@
       <c r="J43" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K43" s="19" t="s">
+      <c r="K43" s="84" t="s">
         <v>494</v>
       </c>
       <c r="L43" s="81">
@@ -6135,7 +6144,7 @@
       <c r="P43" s="24">
         <v>5</v>
       </c>
-      <c r="Q43" s="75" t="s">
+      <c r="Q43" s="85" t="s">
         <v>495</v>
       </c>
       <c r="R43" s="44"/>
@@ -6150,25 +6159,25 @@
       <c r="Y43" s="24">
         <v>2</v>
       </c>
-      <c r="Z43" s="76" t="s">
+      <c r="Z43" s="86" t="s">
         <v>196</v>
       </c>
       <c r="AA43" s="17">
         <v>0.15513360171153148</v>
       </c>
-      <c r="AB43" s="19" t="s">
+      <c r="AB43" s="84" t="s">
         <v>309</v>
       </c>
-      <c r="AC43" s="14" t="s">
+      <c r="AC43" s="83" t="s">
         <v>161</v>
       </c>
-      <c r="AD43" s="63" t="s">
+      <c r="AD43" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="AE43" s="64" t="s">
+      <c r="AE43" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="AF43" s="78" t="s">
+      <c r="AF43" s="87" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6182,7 +6191,7 @@
       <c r="C44" s="14">
         <v>36</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="83" t="s">
         <v>496</v>
       </c>
       <c r="E44" s="17">
@@ -6191,7 +6200,7 @@
       <c r="F44" s="20">
         <v>24</v>
       </c>
-      <c r="G44" s="14" t="s">
+      <c r="G44" s="83" t="s">
         <v>359</v>
       </c>
       <c r="H44" s="17">
@@ -6203,7 +6212,7 @@
       <c r="J44" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K44" s="19" t="s">
+      <c r="K44" s="84" t="s">
         <v>497</v>
       </c>
       <c r="L44" s="81">
@@ -6221,7 +6230,7 @@
       <c r="P44" s="24">
         <v>23</v>
       </c>
-      <c r="Q44" s="75" t="s">
+      <c r="Q44" s="85" t="s">
         <v>498</v>
       </c>
       <c r="R44" s="44"/>
@@ -6236,16 +6245,16 @@
       <c r="Y44" s="24">
         <v>20</v>
       </c>
-      <c r="Z44" s="76" t="s">
+      <c r="Z44" s="86" t="s">
         <v>218</v>
       </c>
       <c r="AA44" s="17">
         <v>0.19657065200369842</v>
       </c>
-      <c r="AB44" s="19" t="s">
+      <c r="AB44" s="84" t="s">
         <v>310</v>
       </c>
-      <c r="AC44" s="14" t="s">
+      <c r="AC44" s="83" t="s">
         <v>162</v>
       </c>
       <c r="AD44" s="63" t="s">
@@ -6268,7 +6277,7 @@
       <c r="C45" s="14">
         <v>12</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="D45" s="83" t="s">
         <v>499</v>
       </c>
       <c r="E45" s="17" t="s">
@@ -6277,7 +6286,7 @@
       <c r="F45" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G45" s="14" t="s">
+      <c r="G45" s="83" t="s">
         <v>360</v>
       </c>
       <c r="H45" s="17">
@@ -6289,7 +6298,7 @@
       <c r="J45" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K45" s="19" t="s">
+      <c r="K45" s="84" t="s">
         <v>500</v>
       </c>
       <c r="L45" s="81">
@@ -6307,7 +6316,7 @@
       <c r="P45" s="24">
         <v>47</v>
       </c>
-      <c r="Q45" s="75" t="s">
+      <c r="Q45" s="85" t="s">
         <v>501</v>
       </c>
       <c r="R45" s="44"/>
@@ -6322,16 +6331,16 @@
       <c r="Y45" s="24">
         <v>50</v>
       </c>
-      <c r="Z45" s="76" t="s">
+      <c r="Z45" s="86" t="s">
         <v>197</v>
       </c>
       <c r="AA45" s="17">
         <v>0.20092887786830402</v>
       </c>
-      <c r="AB45" s="19" t="s">
+      <c r="AB45" s="84" t="s">
         <v>311</v>
       </c>
-      <c r="AC45" s="14" t="s">
+      <c r="AC45" s="83" t="s">
         <v>163</v>
       </c>
       <c r="AD45" s="63" t="s">

</xml_diff>

<commit_message>
did TN through WY!!!!!
</commit_message>
<xml_diff>
--- a/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
+++ b/RE%3a_LC_Atlas_Data/LC (no trachea) for Alex new.xlsx
@@ -1975,7 +1975,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2145,8 +2145,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2166,6 +2164,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="13" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2211,7 +2210,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2497,10 +2495,10 @@
   <dimension ref="A1:AF58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="O26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="N26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AF45" sqref="AF45"/>
+      <selection pane="bottomRight" activeCell="AF54" sqref="AF54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2540,59 +2538,59 @@
   <sheetData>
     <row r="1" spans="1:32" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="96" t="s">
         <v>541</v>
       </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="95" t="s">
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="94" t="s">
         <v>544</v>
       </c>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="98" t="s">
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="97" t="s">
         <v>539</v>
       </c>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="100" t="s">
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="99" t="s">
         <v>539</v>
       </c>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="102" t="s">
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="101" t="s">
         <v>542</v>
       </c>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="103" t="s">
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="104"/>
-      <c r="T1" s="104"/>
-      <c r="U1" s="93" t="s">
+      <c r="S1" s="103"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="V1" s="94"/>
-      <c r="W1" s="94"/>
-      <c r="X1" s="95" t="s">
+      <c r="V1" s="93"/>
+      <c r="W1" s="93"/>
+      <c r="X1" s="94" t="s">
         <v>543</v>
       </c>
-      <c r="Y1" s="96"/>
-      <c r="Z1" s="96"/>
-      <c r="AA1" s="90" t="s">
+      <c r="Y1" s="95"/>
+      <c r="Z1" s="95"/>
+      <c r="AA1" s="89" t="s">
         <v>540</v>
       </c>
-      <c r="AB1" s="91"/>
-      <c r="AC1" s="92"/>
+      <c r="AB1" s="90"/>
+      <c r="AC1" s="91"/>
       <c r="AD1" s="58" t="s">
         <v>123</v>
       </c>
       <c r="AE1" s="59"/>
-      <c r="AF1" s="79"/>
+      <c r="AF1" s="77"/>
     </row>
-    <row r="2" spans="1:32" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2686,7 +2684,7 @@
       <c r="AE2" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="AF2" s="80" t="s">
+      <c r="AF2" s="78" t="s">
         <v>224</v>
       </c>
     </row>
@@ -2741,7 +2739,7 @@
       <c r="AC3" s="62"/>
       <c r="AD3" s="17"/>
       <c r="AE3" s="62"/>
-      <c r="AF3" s="77"/>
+      <c r="AF3" s="75"/>
     </row>
     <row r="4" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -2753,7 +2751,7 @@
       <c r="C4" s="14">
         <v>41</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="81" t="s">
         <v>370</v>
       </c>
       <c r="E4" s="17">
@@ -2762,25 +2760,25 @@
       <c r="F4" s="20">
         <v>30</v>
       </c>
-      <c r="G4" s="83" t="s">
+      <c r="G4" s="81" t="s">
         <v>319</v>
       </c>
-      <c r="H4" s="81">
+      <c r="H4" s="79">
         <v>0.18840000000000001</v>
       </c>
-      <c r="I4" s="82">
+      <c r="I4" s="80">
         <v>0.4516</v>
       </c>
       <c r="J4" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K4" s="84" t="s">
+      <c r="K4" s="82" t="s">
         <v>371</v>
       </c>
-      <c r="L4" s="81">
+      <c r="L4" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M4" s="82">
+      <c r="M4" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N4" s="68" t="s">
@@ -2792,7 +2790,7 @@
       <c r="P4" s="24">
         <v>35</v>
       </c>
-      <c r="Q4" s="85" t="s">
+      <c r="Q4" s="83" t="s">
         <v>372</v>
       </c>
       <c r="R4" s="44"/>
@@ -2807,25 +2805,25 @@
       <c r="Y4" s="24">
         <v>22</v>
       </c>
-      <c r="Z4" s="86" t="s">
+      <c r="Z4" s="84" t="s">
         <v>203</v>
       </c>
       <c r="AA4" s="17">
         <v>0.21404947686126119</v>
       </c>
-      <c r="AB4" s="84" t="s">
+      <c r="AB4" s="82" t="s">
         <v>275</v>
       </c>
-      <c r="AC4" s="83" t="s">
+      <c r="AC4" s="81" t="s">
         <v>127</v>
       </c>
-      <c r="AD4" s="88" t="s">
+      <c r="AD4" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="AE4" s="89" t="s">
+      <c r="AE4" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="AF4" s="87" t="s">
+      <c r="AF4" s="85" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2839,7 +2837,7 @@
       <c r="C5" s="14">
         <v>25</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="81" t="s">
         <v>373</v>
       </c>
       <c r="E5" s="17">
@@ -2848,7 +2846,7 @@
       <c r="F5" s="20">
         <v>22</v>
       </c>
-      <c r="G5" s="83" t="s">
+      <c r="G5" s="81" t="s">
         <v>320</v>
       </c>
       <c r="H5" s="17">
@@ -2860,13 +2858,13 @@
       <c r="J5" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K5" s="84" t="s">
+      <c r="K5" s="82" t="s">
         <v>374</v>
       </c>
-      <c r="L5" s="81">
+      <c r="L5" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M5" s="82">
+      <c r="M5" s="80">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="N5" s="68" t="s">
@@ -2878,7 +2876,7 @@
       <c r="P5" s="24">
         <v>40</v>
       </c>
-      <c r="Q5" s="85" t="s">
+      <c r="Q5" s="83" t="s">
         <v>375</v>
       </c>
       <c r="R5" s="44"/>
@@ -2893,25 +2891,25 @@
       <c r="Y5" s="24">
         <v>28</v>
       </c>
-      <c r="Z5" s="86" t="s">
+      <c r="Z5" s="84" t="s">
         <v>204</v>
       </c>
       <c r="AA5" s="17">
         <v>0.19103082458548165</v>
       </c>
-      <c r="AB5" s="84" t="s">
+      <c r="AB5" s="82" t="s">
         <v>276</v>
       </c>
-      <c r="AC5" s="83" t="s">
+      <c r="AC5" s="81" t="s">
         <v>128</v>
       </c>
-      <c r="AD5" s="88" t="s">
+      <c r="AD5" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="AE5" s="89" t="s">
+      <c r="AE5" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="AF5" s="87" t="s">
+      <c r="AF5" s="85" t="s">
         <v>226</v>
       </c>
     </row>
@@ -2925,7 +2923,7 @@
       <c r="C6" s="14">
         <v>8</v>
       </c>
-      <c r="D6" s="83" t="s">
+      <c r="D6" s="81" t="s">
         <v>376</v>
       </c>
       <c r="E6" s="17">
@@ -2934,7 +2932,7 @@
       <c r="F6" s="20">
         <v>12</v>
       </c>
-      <c r="G6" s="83" t="s">
+      <c r="G6" s="81" t="s">
         <v>321</v>
       </c>
       <c r="H6" s="17">
@@ -2946,13 +2944,13 @@
       <c r="J6" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K6" s="84" t="s">
+      <c r="K6" s="82" t="s">
         <v>377</v>
       </c>
-      <c r="L6" s="81">
+      <c r="L6" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M6" s="82">
+      <c r="M6" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N6" s="68" t="s">
@@ -2964,7 +2962,7 @@
       <c r="P6" s="24">
         <v>38</v>
       </c>
-      <c r="Q6" s="85" t="s">
+      <c r="Q6" s="83" t="s">
         <v>378</v>
       </c>
       <c r="R6" s="44"/>
@@ -2979,25 +2977,25 @@
       <c r="Y6" s="24">
         <v>39</v>
       </c>
-      <c r="Z6" s="86" t="s">
+      <c r="Z6" s="84" t="s">
         <v>173</v>
       </c>
       <c r="AA6" s="17">
         <v>0.14043987546412229</v>
       </c>
-      <c r="AB6" s="84" t="s">
+      <c r="AB6" s="82" t="s">
         <v>277</v>
       </c>
-      <c r="AC6" s="83" t="s">
+      <c r="AC6" s="81" t="s">
         <v>129</v>
       </c>
-      <c r="AD6" s="88" t="s">
+      <c r="AD6" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="AE6" s="89" t="s">
+      <c r="AE6" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="AF6" s="87" t="s">
+      <c r="AF6" s="85" t="s">
         <v>227</v>
       </c>
     </row>
@@ -3011,7 +3009,7 @@
       <c r="C7" s="14">
         <v>49</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="81" t="s">
         <v>379</v>
       </c>
       <c r="E7" s="17" t="s">
@@ -3020,7 +3018,7 @@
       <c r="F7" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="83" t="s">
+      <c r="G7" s="81" t="s">
         <v>322</v>
       </c>
       <c r="H7" s="17">
@@ -3032,13 +3030,13 @@
       <c r="J7" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K7" s="84" t="s">
+      <c r="K7" s="82" t="s">
         <v>382</v>
       </c>
-      <c r="L7" s="81">
+      <c r="L7" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M7" s="82">
+      <c r="M7" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N7" s="68" t="s">
@@ -3050,7 +3048,7 @@
       <c r="P7" s="24">
         <v>32</v>
       </c>
-      <c r="Q7" s="85" t="s">
+      <c r="Q7" s="83" t="s">
         <v>383</v>
       </c>
       <c r="R7" s="44"/>
@@ -3065,25 +3063,25 @@
       <c r="Y7" s="24">
         <v>38</v>
       </c>
-      <c r="Z7" s="86" t="s">
+      <c r="Z7" s="84" t="s">
         <v>174</v>
       </c>
       <c r="AA7" s="17">
         <v>0.24883340581347232</v>
       </c>
-      <c r="AB7" s="84" t="s">
+      <c r="AB7" s="82" t="s">
         <v>380</v>
       </c>
-      <c r="AC7" s="83" t="s">
+      <c r="AC7" s="81" t="s">
         <v>381</v>
       </c>
-      <c r="AD7" s="88" t="s">
+      <c r="AD7" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="AE7" s="89" t="s">
+      <c r="AE7" s="87" t="s">
         <v>78</v>
       </c>
-      <c r="AF7" s="87" t="s">
+      <c r="AF7" s="85" t="s">
         <v>228</v>
       </c>
     </row>
@@ -3097,7 +3095,7 @@
       <c r="C8" s="14">
         <v>4</v>
       </c>
-      <c r="D8" s="83" t="s">
+      <c r="D8" s="81" t="s">
         <v>384</v>
       </c>
       <c r="E8" s="17">
@@ -3106,7 +3104,7 @@
       <c r="F8" s="20">
         <v>10</v>
       </c>
-      <c r="G8" s="83" t="s">
+      <c r="G8" s="81" t="s">
         <v>323</v>
       </c>
       <c r="H8" s="17">
@@ -3118,13 +3116,13 @@
       <c r="J8" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K8" s="84" t="s">
+      <c r="K8" s="82" t="s">
         <v>387</v>
       </c>
-      <c r="L8" s="81">
+      <c r="L8" s="79">
         <v>0.56899999999999995</v>
       </c>
-      <c r="M8" s="82">
+      <c r="M8" s="80">
         <v>0.05</v>
       </c>
       <c r="N8" s="68" t="s">
@@ -3136,7 +3134,7 @@
       <c r="P8" s="24">
         <v>18</v>
       </c>
-      <c r="Q8" s="85" t="s">
+      <c r="Q8" s="83" t="s">
         <v>388</v>
       </c>
       <c r="R8" s="44"/>
@@ -3151,25 +3149,25 @@
       <c r="Y8" s="24">
         <v>45</v>
       </c>
-      <c r="Z8" s="86" t="s">
+      <c r="Z8" s="84" t="s">
         <v>175</v>
       </c>
       <c r="AA8" s="17">
         <v>0.11678356434966665</v>
       </c>
-      <c r="AB8" s="84" t="s">
+      <c r="AB8" s="82" t="s">
         <v>385</v>
       </c>
-      <c r="AC8" s="83" t="s">
+      <c r="AC8" s="81" t="s">
         <v>386</v>
       </c>
-      <c r="AD8" s="88" t="s">
+      <c r="AD8" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="AE8" s="89" t="s">
+      <c r="AE8" s="87" t="s">
         <v>80</v>
       </c>
-      <c r="AF8" s="87" t="s">
+      <c r="AF8" s="85" t="s">
         <v>229</v>
       </c>
     </row>
@@ -3183,7 +3181,7 @@
       <c r="C9" s="14">
         <v>3</v>
       </c>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="81" t="s">
         <v>389</v>
       </c>
       <c r="E9" s="17">
@@ -3192,7 +3190,7 @@
       <c r="F9" s="20">
         <v>6</v>
       </c>
-      <c r="G9" s="83" t="s">
+      <c r="G9" s="81" t="s">
         <v>324</v>
       </c>
       <c r="H9" s="17">
@@ -3204,13 +3202,13 @@
       <c r="J9" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K9" s="84" t="s">
+      <c r="K9" s="82" t="s">
         <v>390</v>
       </c>
-      <c r="L9" s="81">
+      <c r="L9" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M9" s="82">
+      <c r="M9" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N9" s="68" t="s">
@@ -3222,7 +3220,7 @@
       <c r="P9" s="24">
         <v>19</v>
       </c>
-      <c r="Q9" s="85" t="s">
+      <c r="Q9" s="83" t="s">
         <v>391</v>
       </c>
       <c r="R9" s="44"/>
@@ -3237,25 +3235,25 @@
       <c r="Y9" s="24">
         <v>15</v>
       </c>
-      <c r="Z9" s="86" t="s">
+      <c r="Z9" s="84" t="s">
         <v>205</v>
       </c>
       <c r="AA9" s="17">
         <v>0.15647582480563493</v>
       </c>
-      <c r="AB9" s="84" t="s">
+      <c r="AB9" s="82" t="s">
         <v>278</v>
       </c>
-      <c r="AC9" s="83" t="s">
+      <c r="AC9" s="81" t="s">
         <v>130</v>
       </c>
-      <c r="AD9" s="88" t="s">
+      <c r="AD9" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="AE9" s="89" t="s">
+      <c r="AE9" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="AF9" s="87" t="s">
+      <c r="AF9" s="85" t="s">
         <v>230</v>
       </c>
     </row>
@@ -3269,7 +3267,7 @@
       <c r="C10" s="14">
         <v>27</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="81" t="s">
         <v>392</v>
       </c>
       <c r="E10" s="17">
@@ -3278,7 +3276,7 @@
       <c r="F10" s="20">
         <v>2</v>
       </c>
-      <c r="G10" s="83" t="s">
+      <c r="G10" s="81" t="s">
         <v>325</v>
       </c>
       <c r="H10" s="17">
@@ -3290,13 +3288,13 @@
       <c r="J10" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K10" s="84" t="s">
+      <c r="K10" s="82" t="s">
         <v>393</v>
       </c>
-      <c r="L10" s="81">
+      <c r="L10" s="79">
         <v>0.65300000000000002</v>
       </c>
-      <c r="M10" s="82">
+      <c r="M10" s="80">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="N10" s="68" t="s">
@@ -3308,7 +3306,7 @@
       <c r="P10" s="24">
         <v>2</v>
       </c>
-      <c r="Q10" s="85" t="s">
+      <c r="Q10" s="83" t="s">
         <v>394</v>
       </c>
       <c r="R10" s="44"/>
@@ -3323,25 +3321,25 @@
       <c r="Y10" s="24">
         <v>3</v>
       </c>
-      <c r="Z10" s="86" t="s">
+      <c r="Z10" s="84" t="s">
         <v>176</v>
       </c>
       <c r="AA10" s="17">
         <v>0.13481608001043952</v>
       </c>
-      <c r="AB10" s="84" t="s">
+      <c r="AB10" s="82" t="s">
         <v>279</v>
       </c>
-      <c r="AC10" s="83" t="s">
+      <c r="AC10" s="81" t="s">
         <v>131</v>
       </c>
-      <c r="AD10" s="88" t="s">
+      <c r="AD10" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="AE10" s="89" t="s">
+      <c r="AE10" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="AF10" s="87" t="s">
+      <c r="AF10" s="85" t="s">
         <v>231</v>
       </c>
     </row>
@@ -3355,7 +3353,7 @@
       <c r="C11" s="14">
         <v>42</v>
       </c>
-      <c r="D11" s="83" t="s">
+      <c r="D11" s="81" t="s">
         <v>395</v>
       </c>
       <c r="E11" s="17" t="s">
@@ -3364,7 +3362,7 @@
       <c r="F11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="83" t="s">
+      <c r="G11" s="81" t="s">
         <v>326</v>
       </c>
       <c r="H11" s="17">
@@ -3376,13 +3374,13 @@
       <c r="J11" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K11" s="84" t="s">
+      <c r="K11" s="82" t="s">
         <v>396</v>
       </c>
-      <c r="L11" s="81">
+      <c r="L11" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M11" s="82">
+      <c r="M11" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N11" s="68" t="s">
@@ -3394,7 +3392,7 @@
       <c r="P11" s="24">
         <v>34</v>
       </c>
-      <c r="Q11" s="85" t="s">
+      <c r="Q11" s="83" t="s">
         <v>397</v>
       </c>
       <c r="R11" s="44"/>
@@ -3409,25 +3407,25 @@
       <c r="Y11" s="24">
         <v>1</v>
       </c>
-      <c r="Z11" s="86" t="s">
+      <c r="Z11" s="84" t="s">
         <v>177</v>
       </c>
       <c r="AA11" s="17">
         <v>0.17360395746617199</v>
       </c>
-      <c r="AB11" s="84" t="s">
+      <c r="AB11" s="82" t="s">
         <v>280</v>
       </c>
-      <c r="AC11" s="83" t="s">
+      <c r="AC11" s="81" t="s">
         <v>132</v>
       </c>
-      <c r="AD11" s="88" t="s">
+      <c r="AD11" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="AE11" s="89" t="s">
+      <c r="AE11" s="87" t="s">
         <v>85</v>
       </c>
-      <c r="AF11" s="87" t="s">
+      <c r="AF11" s="85" t="s">
         <v>232</v>
       </c>
     </row>
@@ -3441,7 +3439,7 @@
       <c r="C12" s="14">
         <v>17</v>
       </c>
-      <c r="D12" s="83" t="s">
+      <c r="D12" s="81" t="s">
         <v>534</v>
       </c>
       <c r="E12" s="17" t="s">
@@ -3450,7 +3448,7 @@
       <c r="F12" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="83" t="s">
+      <c r="G12" s="81" t="s">
         <v>327</v>
       </c>
       <c r="H12" s="17">
@@ -3462,13 +3460,13 @@
       <c r="J12" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K12" s="84" t="s">
+      <c r="K12" s="82" t="s">
         <v>536</v>
       </c>
-      <c r="L12" s="81">
+      <c r="L12" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M12" s="82">
+      <c r="M12" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N12" s="68" t="s">
@@ -3480,7 +3478,7 @@
       <c r="P12" s="24">
         <v>30</v>
       </c>
-      <c r="Q12" s="85" t="s">
+      <c r="Q12" s="83" t="s">
         <v>537</v>
       </c>
       <c r="R12" s="44"/>
@@ -3495,25 +3493,25 @@
       <c r="Y12" s="24">
         <v>25</v>
       </c>
-      <c r="Z12" s="86" t="s">
+      <c r="Z12" s="84" t="s">
         <v>538</v>
       </c>
       <c r="AA12" s="17">
         <v>0.15994308319695427</v>
       </c>
-      <c r="AB12" s="84" t="s">
+      <c r="AB12" s="82" t="s">
         <v>535</v>
       </c>
-      <c r="AC12" s="83" t="s">
+      <c r="AC12" s="81" t="s">
         <v>273</v>
       </c>
-      <c r="AD12" s="88" t="s">
+      <c r="AD12" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="AE12" s="89" t="s">
+      <c r="AE12" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="AF12" s="87" t="s">
+      <c r="AF12" s="85" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3527,7 +3525,7 @@
       <c r="C13" s="14">
         <v>26</v>
       </c>
-      <c r="D13" s="83" t="s">
+      <c r="D13" s="81" t="s">
         <v>398</v>
       </c>
       <c r="E13" s="17" t="s">
@@ -3536,7 +3534,7 @@
       <c r="F13" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="83" t="s">
+      <c r="G13" s="81" t="s">
         <v>328</v>
       </c>
       <c r="H13" s="17">
@@ -3548,13 +3546,13 @@
       <c r="J13" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K13" s="84" t="s">
+      <c r="K13" s="82" t="s">
         <v>399</v>
       </c>
-      <c r="L13" s="81">
+      <c r="L13" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M13" s="82">
+      <c r="M13" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N13" s="68" t="s">
@@ -3566,7 +3564,7 @@
       <c r="P13" s="24">
         <v>15</v>
       </c>
-      <c r="Q13" s="85" t="s">
+      <c r="Q13" s="83" t="s">
         <v>400</v>
       </c>
       <c r="R13" s="44"/>
@@ -3581,25 +3579,25 @@
       <c r="Y13" s="24">
         <v>21</v>
       </c>
-      <c r="Z13" s="86" t="s">
+      <c r="Z13" s="84" t="s">
         <v>206</v>
       </c>
       <c r="AA13" s="17">
         <v>0.15802004831552136</v>
       </c>
-      <c r="AB13" s="84" t="s">
+      <c r="AB13" s="82" t="s">
         <v>281</v>
       </c>
-      <c r="AC13" s="83" t="s">
+      <c r="AC13" s="81" t="s">
         <v>133</v>
       </c>
-      <c r="AD13" s="88" t="s">
+      <c r="AD13" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="AE13" s="89" t="s">
+      <c r="AE13" s="87" t="s">
         <v>86</v>
       </c>
-      <c r="AF13" s="87" t="s">
+      <c r="AF13" s="85" t="s">
         <v>233</v>
       </c>
     </row>
@@ -3613,7 +3611,7 @@
       <c r="C14" s="14">
         <v>32</v>
       </c>
-      <c r="D14" s="83" t="s">
+      <c r="D14" s="81" t="s">
         <v>401</v>
       </c>
       <c r="E14" s="17">
@@ -3622,7 +3620,7 @@
       <c r="F14" s="20">
         <v>23</v>
       </c>
-      <c r="G14" s="83" t="s">
+      <c r="G14" s="81" t="s">
         <v>329</v>
       </c>
       <c r="H14" s="17">
@@ -3634,13 +3632,13 @@
       <c r="J14" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K14" s="84" t="s">
+      <c r="K14" s="82" t="s">
         <v>402</v>
       </c>
-      <c r="L14" s="81">
+      <c r="L14" s="79">
         <v>0.498</v>
       </c>
-      <c r="M14" s="82">
+      <c r="M14" s="80">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="N14" s="68" t="s">
@@ -3652,7 +3650,7 @@
       <c r="P14" s="24">
         <v>24</v>
       </c>
-      <c r="Q14" s="85" t="s">
+      <c r="Q14" s="83" t="s">
         <v>403</v>
       </c>
       <c r="R14" s="44"/>
@@ -3667,25 +3665,25 @@
       <c r="Y14" s="24">
         <v>31</v>
       </c>
-      <c r="Z14" s="86" t="s">
+      <c r="Z14" s="84" t="s">
         <v>178</v>
       </c>
       <c r="AA14" s="17">
         <v>0.17678297082342789</v>
       </c>
-      <c r="AB14" s="84" t="s">
+      <c r="AB14" s="82" t="s">
         <v>282</v>
       </c>
-      <c r="AC14" s="83" t="s">
+      <c r="AC14" s="81" t="s">
         <v>134</v>
       </c>
-      <c r="AD14" s="88" t="s">
+      <c r="AD14" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="AE14" s="89" t="s">
+      <c r="AE14" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="AF14" s="87" t="s">
+      <c r="AF14" s="85" t="s">
         <v>234</v>
       </c>
     </row>
@@ -3699,7 +3697,7 @@
       <c r="C15" s="14">
         <v>5</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="D15" s="81" t="s">
         <v>404</v>
       </c>
       <c r="E15" s="17">
@@ -3708,7 +3706,7 @@
       <c r="F15" s="20">
         <v>20</v>
       </c>
-      <c r="G15" s="83" t="s">
+      <c r="G15" s="81" t="s">
         <v>330</v>
       </c>
       <c r="H15" s="17">
@@ -3720,13 +3718,13 @@
       <c r="J15" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K15" s="84" t="s">
+      <c r="K15" s="82" t="s">
         <v>405</v>
       </c>
-      <c r="L15" s="81">
+      <c r="L15" s="79">
         <v>0.59199999999999997</v>
       </c>
-      <c r="M15" s="82">
+      <c r="M15" s="80">
         <v>0.06</v>
       </c>
       <c r="N15" s="68" t="s">
@@ -3738,7 +3736,7 @@
       <c r="P15" s="24">
         <v>39</v>
       </c>
-      <c r="Q15" s="85" t="s">
+      <c r="Q15" s="83" t="s">
         <v>406</v>
       </c>
       <c r="R15" s="44"/>
@@ -3753,25 +3751,25 @@
       <c r="Y15" s="24">
         <v>42</v>
       </c>
-      <c r="Z15" s="86" t="s">
+      <c r="Z15" s="84" t="s">
         <v>179</v>
       </c>
       <c r="AA15" s="17">
         <v>0.14093636018627745</v>
       </c>
-      <c r="AB15" s="84" t="s">
+      <c r="AB15" s="82" t="s">
         <v>283</v>
       </c>
-      <c r="AC15" s="83" t="s">
+      <c r="AC15" s="81" t="s">
         <v>135</v>
       </c>
-      <c r="AD15" s="88" t="s">
+      <c r="AD15" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="AE15" s="89" t="s">
+      <c r="AE15" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="AF15" s="87" t="s">
+      <c r="AF15" s="85" t="s">
         <v>235</v>
       </c>
     </row>
@@ -3785,7 +3783,7 @@
       <c r="C16" s="14">
         <v>7</v>
       </c>
-      <c r="D16" s="83" t="s">
+      <c r="D16" s="81" t="s">
         <v>407</v>
       </c>
       <c r="E16" s="17">
@@ -3794,7 +3792,7 @@
       <c r="F16" s="20">
         <v>21</v>
       </c>
-      <c r="G16" s="83" t="s">
+      <c r="G16" s="81" t="s">
         <v>331</v>
       </c>
       <c r="H16" s="17">
@@ -3806,13 +3804,13 @@
       <c r="J16" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="84" t="s">
+      <c r="K16" s="82" t="s">
         <v>408</v>
       </c>
-      <c r="L16" s="81">
+      <c r="L16" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M16" s="82">
+      <c r="M16" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N16" s="68" t="s">
@@ -3824,7 +3822,7 @@
       <c r="P16" s="24">
         <v>29</v>
       </c>
-      <c r="Q16" s="85" t="s">
+      <c r="Q16" s="83" t="s">
         <v>409</v>
       </c>
       <c r="R16" s="44"/>
@@ -3839,25 +3837,25 @@
       <c r="Y16" s="24">
         <v>17</v>
       </c>
-      <c r="Z16" s="86" t="s">
+      <c r="Z16" s="84" t="s">
         <v>207</v>
       </c>
       <c r="AA16" s="17">
         <v>0.13843264085255502</v>
       </c>
-      <c r="AB16" s="84" t="s">
+      <c r="AB16" s="82" t="s">
         <v>284</v>
       </c>
-      <c r="AC16" s="83" t="s">
+      <c r="AC16" s="81" t="s">
         <v>136</v>
       </c>
-      <c r="AD16" s="88" t="s">
+      <c r="AD16" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="AE16" s="89" t="s">
+      <c r="AE16" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="AF16" s="87" t="s">
+      <c r="AF16" s="85" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3871,7 +3869,7 @@
       <c r="C17" s="14">
         <v>35</v>
       </c>
-      <c r="D17" s="83" t="s">
+      <c r="D17" s="81" t="s">
         <v>410</v>
       </c>
       <c r="E17" s="17">
@@ -3880,7 +3878,7 @@
       <c r="F17" s="20">
         <v>7</v>
       </c>
-      <c r="G17" s="83" t="s">
+      <c r="G17" s="81" t="s">
         <v>332</v>
       </c>
       <c r="H17" s="17">
@@ -3892,13 +3890,13 @@
       <c r="J17" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K17" s="84" t="s">
+      <c r="K17" s="82" t="s">
         <v>411</v>
       </c>
-      <c r="L17" s="81">
+      <c r="L17" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M17" s="82">
+      <c r="M17" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N17" s="68" t="s">
@@ -3910,7 +3908,7 @@
       <c r="P17" s="24">
         <v>10</v>
       </c>
-      <c r="Q17" s="85" t="s">
+      <c r="Q17" s="83" t="s">
         <v>412</v>
       </c>
       <c r="R17" s="44"/>
@@ -3925,25 +3923,25 @@
       <c r="Y17" s="24">
         <v>37</v>
       </c>
-      <c r="Z17" s="86" t="s">
+      <c r="Z17" s="84" t="s">
         <v>180</v>
       </c>
       <c r="AA17" s="17">
         <v>0.15129163664581946</v>
       </c>
-      <c r="AB17" s="84" t="s">
+      <c r="AB17" s="82" t="s">
         <v>285</v>
       </c>
-      <c r="AC17" s="83" t="s">
+      <c r="AC17" s="81" t="s">
         <v>137</v>
       </c>
-      <c r="AD17" s="88" t="s">
+      <c r="AD17" s="86" t="s">
         <v>90</v>
       </c>
-      <c r="AE17" s="89" t="s">
+      <c r="AE17" s="87" t="s">
         <v>91</v>
       </c>
-      <c r="AF17" s="87" t="s">
+      <c r="AF17" s="85" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3957,7 +3955,7 @@
       <c r="C18" s="14">
         <v>44</v>
       </c>
-      <c r="D18" s="83" t="s">
+      <c r="D18" s="81" t="s">
         <v>413</v>
       </c>
       <c r="E18" s="17" t="s">
@@ -3966,7 +3964,7 @@
       <c r="F18" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="83" t="s">
+      <c r="G18" s="81" t="s">
         <v>333</v>
       </c>
       <c r="H18" s="17">
@@ -3978,13 +3976,13 @@
       <c r="J18" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K18" s="84" t="s">
+      <c r="K18" s="82" t="s">
         <v>414</v>
       </c>
-      <c r="L18" s="81">
+      <c r="L18" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M18" s="82">
+      <c r="M18" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N18" s="68" t="s">
@@ -3996,7 +3994,7 @@
       <c r="P18" s="24">
         <v>42</v>
       </c>
-      <c r="Q18" s="85" t="s">
+      <c r="Q18" s="83" t="s">
         <v>415</v>
       </c>
       <c r="R18" s="44"/>
@@ -4011,25 +4009,25 @@
       <c r="Y18" s="24">
         <v>12</v>
       </c>
-      <c r="Z18" s="86" t="s">
+      <c r="Z18" s="84" t="s">
         <v>208</v>
       </c>
       <c r="AA18" s="17">
         <v>0.2055285375712991</v>
       </c>
-      <c r="AB18" s="84" t="s">
+      <c r="AB18" s="82" t="s">
         <v>286</v>
       </c>
-      <c r="AC18" s="83" t="s">
+      <c r="AC18" s="81" t="s">
         <v>138</v>
       </c>
-      <c r="AD18" s="88" t="s">
+      <c r="AD18" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="AE18" s="89" t="s">
+      <c r="AE18" s="87" t="s">
         <v>93</v>
       </c>
-      <c r="AF18" s="87" t="s">
+      <c r="AF18" s="85" t="s">
         <v>238</v>
       </c>
     </row>
@@ -4043,7 +4041,7 @@
       <c r="C19" s="14">
         <v>28</v>
       </c>
-      <c r="D19" s="83" t="s">
+      <c r="D19" s="81" t="s">
         <v>416</v>
       </c>
       <c r="E19" s="17">
@@ -4052,7 +4050,7 @@
       <c r="F19" s="20">
         <v>25</v>
       </c>
-      <c r="G19" s="83" t="s">
+      <c r="G19" s="81" t="s">
         <v>334</v>
       </c>
       <c r="H19" s="17">
@@ -4064,13 +4062,13 @@
       <c r="J19" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K19" s="84" t="s">
+      <c r="K19" s="82" t="s">
         <v>417</v>
       </c>
-      <c r="L19" s="81">
+      <c r="L19" s="79">
         <v>0.499</v>
       </c>
-      <c r="M19" s="82">
+      <c r="M19" s="80">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="N19" s="68" t="s">
@@ -4082,7 +4080,7 @@
       <c r="P19" s="24">
         <v>36</v>
       </c>
-      <c r="Q19" s="85" t="s">
+      <c r="Q19" s="83" t="s">
         <v>418</v>
       </c>
       <c r="R19" s="44"/>
@@ -4097,25 +4095,25 @@
       <c r="Y19" s="24">
         <v>24</v>
       </c>
-      <c r="Z19" s="86" t="s">
+      <c r="Z19" s="84" t="s">
         <v>209</v>
       </c>
       <c r="AA19" s="17">
         <v>0.18057406771974777</v>
       </c>
-      <c r="AB19" s="84" t="s">
+      <c r="AB19" s="82" t="s">
         <v>287</v>
       </c>
-      <c r="AC19" s="83" t="s">
+      <c r="AC19" s="81" t="s">
         <v>139</v>
       </c>
-      <c r="AD19" s="88" t="s">
+      <c r="AD19" s="86" t="s">
         <v>94</v>
       </c>
-      <c r="AE19" s="89" t="s">
+      <c r="AE19" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="AF19" s="87" t="s">
+      <c r="AF19" s="85" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4129,7 +4127,7 @@
       <c r="C20" s="14">
         <v>22</v>
       </c>
-      <c r="D20" s="83" t="s">
+      <c r="D20" s="81" t="s">
         <v>419</v>
       </c>
       <c r="E20" s="17" t="s">
@@ -4138,7 +4136,7 @@
       <c r="F20" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="83" t="s">
+      <c r="G20" s="81" t="s">
         <v>335</v>
       </c>
       <c r="H20" s="17">
@@ -4150,13 +4148,13 @@
       <c r="J20" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="K20" s="84" t="s">
+      <c r="K20" s="82" t="s">
         <v>420</v>
       </c>
-      <c r="L20" s="81">
+      <c r="L20" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M20" s="82">
+      <c r="M20" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N20" s="68" t="s">
@@ -4168,7 +4166,7 @@
       <c r="P20" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="Q20" s="85" t="s">
+      <c r="Q20" s="83" t="s">
         <v>421</v>
       </c>
       <c r="R20" s="44"/>
@@ -4183,25 +4181,25 @@
       <c r="Y20" s="24">
         <v>43</v>
       </c>
-      <c r="Z20" s="86" t="s">
+      <c r="Z20" s="84" t="s">
         <v>181</v>
       </c>
       <c r="AA20" s="17">
         <v>0.17715214387576331</v>
       </c>
-      <c r="AB20" s="84" t="s">
+      <c r="AB20" s="82" t="s">
         <v>288</v>
       </c>
-      <c r="AC20" s="83" t="s">
+      <c r="AC20" s="81" t="s">
         <v>140</v>
       </c>
-      <c r="AD20" s="88" t="s">
+      <c r="AD20" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="AE20" s="89" t="s">
+      <c r="AE20" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="AF20" s="87" t="s">
+      <c r="AF20" s="85" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4215,7 +4213,7 @@
       <c r="C21" s="14">
         <v>51</v>
       </c>
-      <c r="D21" s="83" t="s">
+      <c r="D21" s="81" t="s">
         <v>422</v>
       </c>
       <c r="E21" s="17">
@@ -4224,7 +4222,7 @@
       <c r="F21" s="20">
         <v>28</v>
       </c>
-      <c r="G21" s="83" t="s">
+      <c r="G21" s="81" t="s">
         <v>336</v>
       </c>
       <c r="H21" s="17">
@@ -4236,13 +4234,13 @@
       <c r="J21" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K21" s="84" t="s">
+      <c r="K21" s="82" t="s">
         <v>425</v>
       </c>
-      <c r="L21" s="81">
+      <c r="L21" s="79">
         <v>0.48799999999999999</v>
       </c>
-      <c r="M21" s="82">
+      <c r="M21" s="80">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="N21" s="68" t="s">
@@ -4254,7 +4252,7 @@
       <c r="P21" s="24">
         <v>12</v>
       </c>
-      <c r="Q21" s="85" t="s">
+      <c r="Q21" s="83" t="s">
         <v>426</v>
       </c>
       <c r="R21" s="44"/>
@@ -4269,25 +4267,25 @@
       <c r="Y21" s="24">
         <v>7</v>
       </c>
-      <c r="Z21" s="86" t="s">
+      <c r="Z21" s="84" t="s">
         <v>182</v>
       </c>
       <c r="AA21" s="17">
         <v>0.25946109971384973</v>
       </c>
-      <c r="AB21" s="84" t="s">
+      <c r="AB21" s="82" t="s">
         <v>423</v>
       </c>
-      <c r="AC21" s="83" t="s">
+      <c r="AC21" s="81" t="s">
         <v>424</v>
       </c>
-      <c r="AD21" s="88" t="s">
+      <c r="AD21" s="86" t="s">
         <v>97</v>
       </c>
-      <c r="AE21" s="89" t="s">
+      <c r="AE21" s="87" t="s">
         <v>98</v>
       </c>
-      <c r="AF21" s="87" t="s">
+      <c r="AF21" s="85" t="s">
         <v>427</v>
       </c>
     </row>
@@ -4301,7 +4299,7 @@
       <c r="C22" s="14">
         <v>43</v>
       </c>
-      <c r="D22" s="83" t="s">
+      <c r="D22" s="81" t="s">
         <v>428</v>
       </c>
       <c r="E22" s="17">
@@ -4310,7 +4308,7 @@
       <c r="F22" s="20">
         <v>31</v>
       </c>
-      <c r="G22" s="83" t="s">
+      <c r="G22" s="81" t="s">
         <v>337</v>
       </c>
       <c r="H22" s="17">
@@ -4322,13 +4320,13 @@
       <c r="J22" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K22" s="84" t="s">
+      <c r="K22" s="82" t="s">
         <v>429</v>
       </c>
-      <c r="L22" s="81">
+      <c r="L22" s="79">
         <v>0.41</v>
       </c>
-      <c r="M22" s="82">
+      <c r="M22" s="80">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="N22" s="68" t="s">
@@ -4340,7 +4338,7 @@
       <c r="P22" s="24">
         <v>43</v>
       </c>
-      <c r="Q22" s="85" t="s">
+      <c r="Q22" s="83" t="s">
         <v>430</v>
       </c>
       <c r="R22" s="44"/>
@@ -4355,25 +4353,25 @@
       <c r="Y22" s="24">
         <v>35</v>
       </c>
-      <c r="Z22" s="86" t="s">
+      <c r="Z22" s="84" t="s">
         <v>183</v>
       </c>
       <c r="AA22" s="17">
         <v>0.21877266061966386</v>
       </c>
-      <c r="AB22" s="84" t="s">
+      <c r="AB22" s="82" t="s">
         <v>289</v>
       </c>
-      <c r="AC22" s="83" t="s">
+      <c r="AC22" s="81" t="s">
         <v>141</v>
       </c>
-      <c r="AD22" s="88" t="s">
+      <c r="AD22" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="AE22" s="89" t="s">
+      <c r="AE22" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="AF22" s="87" t="s">
+      <c r="AF22" s="85" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4387,7 +4385,7 @@
       <c r="C23" s="14">
         <v>45</v>
       </c>
-      <c r="D23" s="83" t="s">
+      <c r="D23" s="81" t="s">
         <v>431</v>
       </c>
       <c r="E23" s="17">
@@ -4396,7 +4394,7 @@
       <c r="F23" s="20">
         <v>10</v>
       </c>
-      <c r="G23" s="83" t="s">
+      <c r="G23" s="81" t="s">
         <v>338</v>
       </c>
       <c r="H23" s="17">
@@ -4408,13 +4406,13 @@
       <c r="J23" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K23" s="84" t="s">
+      <c r="K23" s="82" t="s">
         <v>432</v>
       </c>
-      <c r="L23" s="81">
+      <c r="L23" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M23" s="82">
+      <c r="M23" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N23" s="68" t="s">
@@ -4426,7 +4424,7 @@
       <c r="P23" s="24">
         <v>13</v>
       </c>
-      <c r="Q23" s="85" t="s">
+      <c r="Q23" s="83" t="s">
         <v>433</v>
       </c>
       <c r="R23" s="44"/>
@@ -4441,25 +4439,25 @@
       <c r="Y23" s="24">
         <v>23</v>
       </c>
-      <c r="Z23" s="86" t="s">
+      <c r="Z23" s="84" t="s">
         <v>210</v>
       </c>
       <c r="AA23" s="17">
         <v>0.19465813663811302</v>
       </c>
-      <c r="AB23" s="84" t="s">
+      <c r="AB23" s="82" t="s">
         <v>290</v>
       </c>
-      <c r="AC23" s="83" t="s">
+      <c r="AC23" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="AD23" s="88" t="s">
+      <c r="AD23" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="AE23" s="89" t="s">
+      <c r="AE23" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="AF23" s="87" t="s">
+      <c r="AF23" s="85" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4473,7 +4471,7 @@
       <c r="C24" s="14">
         <v>15</v>
       </c>
-      <c r="D24" s="83" t="s">
+      <c r="D24" s="81" t="s">
         <v>434</v>
       </c>
       <c r="E24" s="17" t="s">
@@ -4482,7 +4480,7 @@
       <c r="F24" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="83" t="s">
+      <c r="G24" s="81" t="s">
         <v>339</v>
       </c>
       <c r="H24" s="17">
@@ -4494,13 +4492,13 @@
       <c r="J24" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K24" s="84" t="s">
+      <c r="K24" s="82" t="s">
         <v>435</v>
       </c>
-      <c r="L24" s="81">
+      <c r="L24" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M24" s="82">
+      <c r="M24" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N24" s="68" t="s">
@@ -4512,7 +4510,7 @@
       <c r="P24" s="24">
         <v>8</v>
       </c>
-      <c r="Q24" s="85" t="s">
+      <c r="Q24" s="83" t="s">
         <v>436</v>
       </c>
       <c r="R24" s="44"/>
@@ -4527,25 +4525,25 @@
       <c r="Y24" s="24">
         <v>13</v>
       </c>
-      <c r="Z24" s="86" t="s">
+      <c r="Z24" s="84" t="s">
         <v>211</v>
       </c>
       <c r="AA24" s="17">
         <v>0.15117214410405386</v>
       </c>
-      <c r="AB24" s="84" t="s">
+      <c r="AB24" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="AC24" s="83" t="s">
+      <c r="AC24" s="81" t="s">
         <v>143</v>
       </c>
-      <c r="AD24" s="88" t="s">
+      <c r="AD24" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="AE24" s="89" t="s">
+      <c r="AE24" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="AF24" s="87" t="s">
+      <c r="AF24" s="85" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4559,7 +4557,7 @@
       <c r="C25" s="14">
         <v>29</v>
       </c>
-      <c r="D25" s="83" t="s">
+      <c r="D25" s="81" t="s">
         <v>437</v>
       </c>
       <c r="E25" s="17" t="s">
@@ -4568,7 +4566,7 @@
       <c r="F25" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="83" t="s">
+      <c r="G25" s="81" t="s">
         <v>340</v>
       </c>
       <c r="H25" s="17">
@@ -4580,13 +4578,13 @@
       <c r="J25" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K25" s="84" t="s">
+      <c r="K25" s="82" t="s">
         <v>438</v>
       </c>
-      <c r="L25" s="81">
+      <c r="L25" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M25" s="82">
+      <c r="M25" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N25" s="68" t="s">
@@ -4598,7 +4596,7 @@
       <c r="P25" s="24">
         <v>1</v>
       </c>
-      <c r="Q25" s="85" t="s">
+      <c r="Q25" s="83" t="s">
         <v>439</v>
       </c>
       <c r="R25" s="44"/>
@@ -4613,25 +4611,25 @@
       <c r="Y25" s="24">
         <v>8</v>
       </c>
-      <c r="Z25" s="86" t="s">
+      <c r="Z25" s="84" t="s">
         <v>184</v>
       </c>
       <c r="AA25" s="17">
         <v>0.13991918454929686</v>
       </c>
-      <c r="AB25" s="84" t="s">
+      <c r="AB25" s="82" t="s">
         <v>292</v>
       </c>
-      <c r="AC25" s="83" t="s">
+      <c r="AC25" s="81" t="s">
         <v>144</v>
       </c>
-      <c r="AD25" s="88" t="s">
+      <c r="AD25" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="AE25" s="89" t="s">
+      <c r="AE25" s="87" t="s">
         <v>100</v>
       </c>
-      <c r="AF25" s="87" t="s">
+      <c r="AF25" s="85" t="s">
         <v>244</v>
       </c>
     </row>
@@ -4645,7 +4643,7 @@
       <c r="C26" s="14">
         <v>33</v>
       </c>
-      <c r="D26" s="83" t="s">
+      <c r="D26" s="81" t="s">
         <v>440</v>
       </c>
       <c r="E26" s="17" t="s">
@@ -4654,7 +4652,7 @@
       <c r="F26" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G26" s="83" t="s">
+      <c r="G26" s="81" t="s">
         <v>341</v>
       </c>
       <c r="H26" s="17">
@@ -4666,13 +4664,13 @@
       <c r="J26" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K26" s="84" t="s">
+      <c r="K26" s="82" t="s">
         <v>441</v>
       </c>
-      <c r="L26" s="81">
+      <c r="L26" s="79">
         <v>0.56299999999999994</v>
       </c>
-      <c r="M26" s="82">
+      <c r="M26" s="80">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="N26" s="68" t="s">
@@ -4684,7 +4682,7 @@
       <c r="P26" s="24">
         <v>25</v>
       </c>
-      <c r="Q26" s="85" t="s">
+      <c r="Q26" s="83" t="s">
         <v>442</v>
       </c>
       <c r="R26" s="44"/>
@@ -4699,25 +4697,25 @@
       <c r="Y26" s="24">
         <v>18</v>
       </c>
-      <c r="Z26" s="86" t="s">
+      <c r="Z26" s="84" t="s">
         <v>212</v>
       </c>
       <c r="AA26" s="17">
         <v>0.20702453871969223</v>
       </c>
-      <c r="AB26" s="84" t="s">
+      <c r="AB26" s="82" t="s">
         <v>293</v>
       </c>
-      <c r="AC26" s="83" t="s">
+      <c r="AC26" s="81" t="s">
         <v>145</v>
       </c>
-      <c r="AD26" s="88" t="s">
+      <c r="AD26" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="AE26" s="89" t="s">
+      <c r="AE26" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="AF26" s="87" t="s">
+      <c r="AF26" s="85" t="s">
         <v>245</v>
       </c>
     </row>
@@ -4731,7 +4729,7 @@
       <c r="C27" s="14">
         <v>9</v>
       </c>
-      <c r="D27" s="83" t="s">
+      <c r="D27" s="81" t="s">
         <v>443</v>
       </c>
       <c r="E27" s="17" t="s">
@@ -4740,7 +4738,7 @@
       <c r="F27" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="83" t="s">
+      <c r="G27" s="81" t="s">
         <v>342</v>
       </c>
       <c r="H27" s="17">
@@ -4752,13 +4750,13 @@
       <c r="J27" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="K27" s="84" t="s">
+      <c r="K27" s="82" t="s">
         <v>444</v>
       </c>
-      <c r="L27" s="81">
+      <c r="L27" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M27" s="82">
+      <c r="M27" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N27" s="68" t="s">
@@ -4770,7 +4768,7 @@
       <c r="P27" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="Q27" s="85" t="s">
+      <c r="Q27" s="83" t="s">
         <v>445</v>
       </c>
       <c r="R27" s="44"/>
@@ -4785,25 +4783,25 @@
       <c r="Y27" s="24">
         <v>34</v>
       </c>
-      <c r="Z27" s="86" t="s">
+      <c r="Z27" s="84" t="s">
         <v>185</v>
       </c>
       <c r="AA27" s="17">
         <v>0.16206774202352683</v>
       </c>
-      <c r="AB27" s="84" t="s">
+      <c r="AB27" s="82" t="s">
         <v>294</v>
       </c>
-      <c r="AC27" s="83" t="s">
+      <c r="AC27" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="AD27" s="88" t="s">
+      <c r="AD27" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="AE27" s="89" t="s">
+      <c r="AE27" s="87" t="s">
         <v>88</v>
       </c>
-      <c r="AF27" s="87" t="s">
+      <c r="AF27" s="85" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4817,7 +4815,7 @@
       <c r="C28" s="14">
         <v>47</v>
       </c>
-      <c r="D28" s="83" t="s">
+      <c r="D28" s="81" t="s">
         <v>446</v>
       </c>
       <c r="E28" s="17">
@@ -4826,7 +4824,7 @@
       <c r="F28" s="20">
         <v>28</v>
       </c>
-      <c r="G28" s="83" t="s">
+      <c r="G28" s="81" t="s">
         <v>343</v>
       </c>
       <c r="H28" s="17">
@@ -4838,13 +4836,13 @@
       <c r="J28" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K28" s="84" t="s">
+      <c r="K28" s="82" t="s">
         <v>449</v>
       </c>
-      <c r="L28" s="81">
+      <c r="L28" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M28" s="82">
+      <c r="M28" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N28" s="68" t="s">
@@ -4856,7 +4854,7 @@
       <c r="P28" s="24">
         <v>41</v>
       </c>
-      <c r="Q28" s="85" t="s">
+      <c r="Q28" s="83" t="s">
         <v>450</v>
       </c>
       <c r="R28" s="44"/>
@@ -4871,25 +4869,25 @@
       <c r="Y28" s="24">
         <v>29</v>
       </c>
-      <c r="Z28" s="86" t="s">
+      <c r="Z28" s="84" t="s">
         <v>213</v>
       </c>
       <c r="AA28" s="17">
         <v>0.22546283216479387</v>
       </c>
-      <c r="AB28" s="84" t="s">
+      <c r="AB28" s="82" t="s">
         <v>447</v>
       </c>
-      <c r="AC28" s="83" t="s">
+      <c r="AC28" s="81" t="s">
         <v>448</v>
       </c>
-      <c r="AD28" s="88" t="s">
+      <c r="AD28" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="AE28" s="89" t="s">
+      <c r="AE28" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="AF28" s="87" t="s">
+      <c r="AF28" s="85" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4903,7 +4901,7 @@
       <c r="C29" s="14">
         <v>46</v>
       </c>
-      <c r="D29" s="83" t="s">
+      <c r="D29" s="81" t="s">
         <v>451</v>
       </c>
       <c r="E29" s="17" t="s">
@@ -4912,7 +4910,7 @@
       <c r="F29" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G29" s="83" t="s">
+      <c r="G29" s="81" t="s">
         <v>344</v>
       </c>
       <c r="H29" s="17">
@@ -4924,13 +4922,13 @@
       <c r="J29" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K29" s="84" t="s">
+      <c r="K29" s="82" t="s">
         <v>452</v>
       </c>
-      <c r="L29" s="81">
+      <c r="L29" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M29" s="82">
+      <c r="M29" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N29" s="68" t="s">
@@ -4942,7 +4940,7 @@
       <c r="P29" s="24">
         <v>27</v>
       </c>
-      <c r="Q29" s="85" t="s">
+      <c r="Q29" s="83" t="s">
         <v>453</v>
       </c>
       <c r="R29" s="44"/>
@@ -4957,25 +4955,25 @@
       <c r="Y29" s="24">
         <v>26</v>
       </c>
-      <c r="Z29" s="86" t="s">
+      <c r="Z29" s="84" t="s">
         <v>214</v>
       </c>
       <c r="AA29" s="17">
         <v>0.22256552446865413</v>
       </c>
-      <c r="AB29" s="84" t="s">
+      <c r="AB29" s="82" t="s">
         <v>295</v>
       </c>
-      <c r="AC29" s="83" t="s">
+      <c r="AC29" s="81" t="s">
         <v>147</v>
       </c>
-      <c r="AD29" s="88" t="s">
+      <c r="AD29" s="86" t="s">
         <v>103</v>
       </c>
-      <c r="AE29" s="89" t="s">
+      <c r="AE29" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="AF29" s="87" t="s">
+      <c r="AF29" s="85" t="s">
         <v>248</v>
       </c>
     </row>
@@ -4989,7 +4987,7 @@
       <c r="C30" s="14">
         <v>13</v>
       </c>
-      <c r="D30" s="83" t="s">
+      <c r="D30" s="81" t="s">
         <v>454</v>
       </c>
       <c r="E30" s="17">
@@ -4998,7 +4996,7 @@
       <c r="F30" s="20">
         <v>13</v>
       </c>
-      <c r="G30" s="83" t="s">
+      <c r="G30" s="81" t="s">
         <v>345</v>
       </c>
       <c r="H30" s="17">
@@ -5010,13 +5008,13 @@
       <c r="J30" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K30" s="84" t="s">
+      <c r="K30" s="82" t="s">
         <v>455</v>
       </c>
-      <c r="L30" s="81">
+      <c r="L30" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M30" s="82">
+      <c r="M30" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N30" s="68" t="s">
@@ -5028,7 +5026,7 @@
       <c r="P30" s="24">
         <v>31</v>
       </c>
-      <c r="Q30" s="85" t="s">
+      <c r="Q30" s="83" t="s">
         <v>456</v>
       </c>
       <c r="R30" s="44"/>
@@ -5043,25 +5041,25 @@
       <c r="Y30" s="24">
         <v>46</v>
       </c>
-      <c r="Z30" s="86" t="s">
+      <c r="Z30" s="84" t="s">
         <v>186</v>
       </c>
       <c r="AA30" s="17">
         <v>0.18910416661379192</v>
       </c>
-      <c r="AB30" s="84" t="s">
+      <c r="AB30" s="82" t="s">
         <v>296</v>
       </c>
-      <c r="AC30" s="83" t="s">
+      <c r="AC30" s="81" t="s">
         <v>148</v>
       </c>
-      <c r="AD30" s="88" t="s">
+      <c r="AD30" s="86" t="s">
         <v>105</v>
       </c>
-      <c r="AE30" s="89" t="s">
+      <c r="AE30" s="87" t="s">
         <v>106</v>
       </c>
-      <c r="AF30" s="87" t="s">
+      <c r="AF30" s="85" t="s">
         <v>249</v>
       </c>
     </row>
@@ -5075,7 +5073,7 @@
       <c r="C31" s="14">
         <v>14</v>
       </c>
-      <c r="D31" s="83" t="s">
+      <c r="D31" s="81" t="s">
         <v>457</v>
       </c>
       <c r="E31" s="17">
@@ -5084,7 +5082,7 @@
       <c r="F31" s="20">
         <v>15</v>
       </c>
-      <c r="G31" s="83" t="s">
+      <c r="G31" s="81" t="s">
         <v>346</v>
       </c>
       <c r="H31" s="17">
@@ -5096,13 +5094,13 @@
       <c r="J31" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K31" s="84" t="s">
+      <c r="K31" s="82" t="s">
         <v>458</v>
       </c>
-      <c r="L31" s="81">
+      <c r="L31" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M31" s="82">
+      <c r="M31" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N31" s="68" t="s">
@@ -5114,7 +5112,7 @@
       <c r="P31" s="24">
         <v>17</v>
       </c>
-      <c r="Q31" s="85" t="s">
+      <c r="Q31" s="83" t="s">
         <v>459</v>
       </c>
       <c r="R31" s="44"/>
@@ -5129,25 +5127,25 @@
       <c r="Y31" s="24">
         <v>40</v>
       </c>
-      <c r="Z31" s="86" t="s">
+      <c r="Z31" s="84" t="s">
         <v>187</v>
       </c>
       <c r="AA31" s="17">
         <v>0.17099298388282824</v>
       </c>
-      <c r="AB31" s="84" t="s">
+      <c r="AB31" s="82" t="s">
         <v>297</v>
       </c>
-      <c r="AC31" s="83" t="s">
+      <c r="AC31" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="AD31" s="88" t="s">
+      <c r="AD31" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="AE31" s="89" t="s">
+      <c r="AE31" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="AF31" s="87" t="s">
+      <c r="AF31" s="85" t="s">
         <v>250</v>
       </c>
     </row>
@@ -5161,7 +5159,7 @@
       <c r="C32" s="14">
         <v>24</v>
       </c>
-      <c r="D32" s="83" t="s">
+      <c r="D32" s="81" t="s">
         <v>460</v>
       </c>
       <c r="E32" s="17" t="s">
@@ -5170,7 +5168,7 @@
       <c r="F32" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="83" t="s">
+      <c r="G32" s="81" t="s">
         <v>347</v>
       </c>
       <c r="H32" s="17">
@@ -5182,13 +5180,13 @@
       <c r="J32" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K32" s="84" t="s">
+      <c r="K32" s="82" t="s">
         <v>461</v>
       </c>
-      <c r="L32" s="81">
+      <c r="L32" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M32" s="82">
+      <c r="M32" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N32" s="68" t="s">
@@ -5200,7 +5198,7 @@
       <c r="P32" s="24">
         <v>37</v>
       </c>
-      <c r="Q32" s="85" t="s">
+      <c r="Q32" s="83" t="s">
         <v>462</v>
       </c>
       <c r="R32" s="44"/>
@@ -5215,25 +5213,25 @@
       <c r="Y32" s="24">
         <v>19</v>
       </c>
-      <c r="Z32" s="86" t="s">
+      <c r="Z32" s="84" t="s">
         <v>215</v>
       </c>
       <c r="AA32" s="17">
         <v>0.17547927543080832</v>
       </c>
-      <c r="AB32" s="84" t="s">
+      <c r="AB32" s="82" t="s">
         <v>298</v>
       </c>
-      <c r="AC32" s="83" t="s">
+      <c r="AC32" s="81" t="s">
         <v>150</v>
       </c>
-      <c r="AD32" s="88" t="s">
+      <c r="AD32" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="AE32" s="89" t="s">
+      <c r="AE32" s="87" t="s">
         <v>106</v>
       </c>
-      <c r="AF32" s="87" t="s">
+      <c r="AF32" s="85" t="s">
         <v>251</v>
       </c>
     </row>
@@ -5247,7 +5245,7 @@
       <c r="C33" s="14">
         <v>34</v>
       </c>
-      <c r="D33" s="83" t="s">
+      <c r="D33" s="81" t="s">
         <v>463</v>
       </c>
       <c r="E33" s="17">
@@ -5256,7 +5254,7 @@
       <c r="F33" s="20">
         <v>3</v>
       </c>
-      <c r="G33" s="83" t="s">
+      <c r="G33" s="81" t="s">
         <v>348</v>
       </c>
       <c r="H33" s="17">
@@ -5268,13 +5266,13 @@
       <c r="J33" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K33" s="84" t="s">
+      <c r="K33" s="82" t="s">
         <v>464</v>
       </c>
-      <c r="L33" s="81">
+      <c r="L33" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M33" s="82">
+      <c r="M33" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N33" s="68" t="s">
@@ -5286,7 +5284,7 @@
       <c r="P33" s="24">
         <v>6</v>
       </c>
-      <c r="Q33" s="85" t="s">
+      <c r="Q33" s="83" t="s">
         <v>465</v>
       </c>
       <c r="R33" s="44"/>
@@ -5301,25 +5299,25 @@
       <c r="Y33" s="24">
         <v>5</v>
       </c>
-      <c r="Z33" s="86" t="s">
+      <c r="Z33" s="84" t="s">
         <v>188</v>
       </c>
       <c r="AA33" s="17">
         <v>0.15908732269244483</v>
       </c>
-      <c r="AB33" s="84" t="s">
+      <c r="AB33" s="82" t="s">
         <v>299</v>
       </c>
-      <c r="AC33" s="83" t="s">
+      <c r="AC33" s="81" t="s">
         <v>151</v>
       </c>
-      <c r="AD33" s="88" t="s">
+      <c r="AD33" s="86" t="s">
         <v>85</v>
       </c>
-      <c r="AE33" s="89" t="s">
+      <c r="AE33" s="87" t="s">
         <v>86</v>
       </c>
-      <c r="AF33" s="87" t="s">
+      <c r="AF33" s="85" t="s">
         <v>252</v>
       </c>
     </row>
@@ -5333,7 +5331,7 @@
       <c r="C34" s="14">
         <v>16</v>
       </c>
-      <c r="D34" s="83" t="s">
+      <c r="D34" s="81" t="s">
         <v>466</v>
       </c>
       <c r="E34" s="17">
@@ -5342,7 +5340,7 @@
       <c r="F34" s="20">
         <v>4</v>
       </c>
-      <c r="G34" s="83" t="s">
+      <c r="G34" s="81" t="s">
         <v>349</v>
       </c>
       <c r="H34" s="17">
@@ -5354,13 +5352,13 @@
       <c r="J34" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K34" s="84" t="s">
+      <c r="K34" s="82" t="s">
         <v>467</v>
       </c>
-      <c r="L34" s="81">
+      <c r="L34" s="79">
         <v>0.64700000000000002</v>
       </c>
-      <c r="M34" s="82">
+      <c r="M34" s="80">
         <v>4.7E-2</v>
       </c>
       <c r="N34" s="68"/>
@@ -5370,7 +5368,7 @@
       <c r="P34" s="24">
         <v>4</v>
       </c>
-      <c r="Q34" s="85" t="s">
+      <c r="Q34" s="83" t="s">
         <v>468</v>
       </c>
       <c r="R34" s="44"/>
@@ -5385,25 +5383,25 @@
       <c r="Y34" s="24">
         <v>4</v>
       </c>
-      <c r="Z34" s="86" t="s">
+      <c r="Z34" s="84" t="s">
         <v>189</v>
       </c>
       <c r="AA34" s="17">
         <v>0.13529447263799368</v>
       </c>
-      <c r="AB34" s="84" t="s">
+      <c r="AB34" s="82" t="s">
         <v>300</v>
       </c>
-      <c r="AC34" s="83" t="s">
+      <c r="AC34" s="81" t="s">
         <v>152</v>
       </c>
-      <c r="AD34" s="88" t="s">
+      <c r="AD34" s="86" t="s">
         <v>106</v>
       </c>
-      <c r="AE34" s="89" t="s">
+      <c r="AE34" s="87" t="s">
         <v>103</v>
       </c>
-      <c r="AF34" s="87" t="s">
+      <c r="AF34" s="85" t="s">
         <v>253</v>
       </c>
     </row>
@@ -5417,7 +5415,7 @@
       <c r="C35" s="14">
         <v>2</v>
       </c>
-      <c r="D35" s="83" t="s">
+      <c r="D35" s="81" t="s">
         <v>469</v>
       </c>
       <c r="E35" s="17">
@@ -5426,7 +5424,7 @@
       <c r="F35" s="20">
         <v>26</v>
       </c>
-      <c r="G35" s="83" t="s">
+      <c r="G35" s="81" t="s">
         <v>350</v>
       </c>
       <c r="H35" s="17">
@@ -5438,13 +5436,13 @@
       <c r="J35" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K35" s="84" t="s">
+      <c r="K35" s="82" t="s">
         <v>470</v>
       </c>
-      <c r="L35" s="81">
+      <c r="L35" s="79">
         <v>0.48699999999999999</v>
       </c>
-      <c r="M35" s="82">
+      <c r="M35" s="80">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="N35" s="68" t="s">
@@ -5456,7 +5454,7 @@
       <c r="P35" s="24">
         <v>46</v>
       </c>
-      <c r="Q35" s="85" t="s">
+      <c r="Q35" s="83" t="s">
         <v>471</v>
       </c>
       <c r="R35" s="44"/>
@@ -5471,25 +5469,25 @@
       <c r="Y35" s="24">
         <v>47</v>
       </c>
-      <c r="Z35" s="86" t="s">
+      <c r="Z35" s="84" t="s">
         <v>190</v>
       </c>
       <c r="AA35" s="17">
         <v>0.1752603184894628</v>
       </c>
-      <c r="AB35" s="84" t="s">
+      <c r="AB35" s="82" t="s">
         <v>301</v>
       </c>
-      <c r="AC35" s="83" t="s">
+      <c r="AC35" s="81" t="s">
         <v>153</v>
       </c>
-      <c r="AD35" s="88" t="s">
+      <c r="AD35" s="86" t="s">
         <v>106</v>
       </c>
-      <c r="AE35" s="89" t="s">
+      <c r="AE35" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="AF35" s="87" t="s">
+      <c r="AF35" s="85" t="s">
         <v>254</v>
       </c>
     </row>
@@ -5503,7 +5501,7 @@
       <c r="C36" s="14">
         <v>21</v>
       </c>
-      <c r="D36" s="83" t="s">
+      <c r="D36" s="81" t="s">
         <v>472</v>
       </c>
       <c r="E36" s="17">
@@ -5512,7 +5510,7 @@
       <c r="F36" s="20">
         <v>1</v>
       </c>
-      <c r="G36" s="83" t="s">
+      <c r="G36" s="81" t="s">
         <v>351</v>
       </c>
       <c r="H36" s="17">
@@ -5524,13 +5522,13 @@
       <c r="J36" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K36" s="84" t="s">
+      <c r="K36" s="82" t="s">
         <v>473</v>
       </c>
-      <c r="L36" s="81">
+      <c r="L36" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M36" s="82">
+      <c r="M36" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N36" s="68" t="s">
@@ -5542,7 +5540,7 @@
       <c r="P36" s="24">
         <v>3</v>
       </c>
-      <c r="Q36" s="85" t="s">
+      <c r="Q36" s="83" t="s">
         <v>474</v>
       </c>
       <c r="R36" s="44"/>
@@ -5557,25 +5555,25 @@
       <c r="Y36" s="24">
         <v>10</v>
       </c>
-      <c r="Z36" s="86" t="s">
+      <c r="Z36" s="84" t="s">
         <v>216</v>
       </c>
       <c r="AA36" s="17">
         <v>0.15219249928945883</v>
       </c>
-      <c r="AB36" s="84" t="s">
+      <c r="AB36" s="82" t="s">
         <v>302</v>
       </c>
-      <c r="AC36" s="83" t="s">
+      <c r="AC36" s="81" t="s">
         <v>154</v>
       </c>
-      <c r="AD36" s="88" t="s">
+      <c r="AD36" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="AE36" s="89" t="s">
+      <c r="AE36" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="AF36" s="87" t="s">
+      <c r="AF36" s="85" t="s">
         <v>255</v>
       </c>
     </row>
@@ -5589,7 +5587,7 @@
       <c r="C37" s="14">
         <v>38</v>
       </c>
-      <c r="D37" s="83" t="s">
+      <c r="D37" s="81" t="s">
         <v>475</v>
       </c>
       <c r="E37" s="17">
@@ -5598,7 +5596,7 @@
       <c r="F37" s="20">
         <v>17</v>
       </c>
-      <c r="G37" s="83" t="s">
+      <c r="G37" s="81" t="s">
         <v>352</v>
       </c>
       <c r="H37" s="17">
@@ -5610,13 +5608,13 @@
       <c r="J37" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K37" s="84" t="s">
+      <c r="K37" s="82" t="s">
         <v>476</v>
       </c>
-      <c r="L37" s="81">
+      <c r="L37" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M37" s="82">
+      <c r="M37" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N37" s="68" t="s">
@@ -5628,7 +5626,7 @@
       <c r="P37" s="24">
         <v>21</v>
       </c>
-      <c r="Q37" s="85" t="s">
+      <c r="Q37" s="83" t="s">
         <v>477</v>
       </c>
       <c r="R37" s="44"/>
@@ -5643,25 +5641,25 @@
       <c r="Y37" s="24">
         <v>14</v>
       </c>
-      <c r="Z37" s="86" t="s">
+      <c r="Z37" s="84" t="s">
         <v>217</v>
       </c>
       <c r="AA37" s="17">
         <v>0.18993389204543945</v>
       </c>
-      <c r="AB37" s="84" t="s">
+      <c r="AB37" s="82" t="s">
         <v>303</v>
       </c>
-      <c r="AC37" s="83" t="s">
+      <c r="AC37" s="81" t="s">
         <v>155</v>
       </c>
-      <c r="AD37" s="88" t="s">
+      <c r="AD37" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="AE37" s="89" t="s">
+      <c r="AE37" s="87" t="s">
         <v>111</v>
       </c>
-      <c r="AF37" s="87" t="s">
+      <c r="AF37" s="85" t="s">
         <v>256</v>
       </c>
     </row>
@@ -5675,7 +5673,7 @@
       <c r="C38" s="14">
         <v>11</v>
       </c>
-      <c r="D38" s="83" t="s">
+      <c r="D38" s="81" t="s">
         <v>478</v>
       </c>
       <c r="E38" s="17">
@@ -5684,7 +5682,7 @@
       <c r="F38" s="20">
         <v>8</v>
       </c>
-      <c r="G38" s="83" t="s">
+      <c r="G38" s="81" t="s">
         <v>353</v>
       </c>
       <c r="H38" s="17">
@@ -5696,13 +5694,13 @@
       <c r="J38" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K38" s="84" t="s">
+      <c r="K38" s="82" t="s">
         <v>479</v>
       </c>
-      <c r="L38" s="81">
+      <c r="L38" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M38" s="82">
+      <c r="M38" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N38" s="68" t="s">
@@ -5714,7 +5712,7 @@
       <c r="P38" s="24">
         <v>14</v>
       </c>
-      <c r="Q38" s="85" t="s">
+      <c r="Q38" s="83" t="s">
         <v>480</v>
       </c>
       <c r="R38" s="44"/>
@@ -5729,25 +5727,25 @@
       <c r="Y38" s="24">
         <v>44</v>
       </c>
-      <c r="Z38" s="86" t="s">
+      <c r="Z38" s="84" t="s">
         <v>191</v>
       </c>
       <c r="AA38" s="17">
         <v>0.18714265521749884</v>
       </c>
-      <c r="AB38" s="84" t="s">
+      <c r="AB38" s="82" t="s">
         <v>304</v>
       </c>
-      <c r="AC38" s="83" t="s">
+      <c r="AC38" s="81" t="s">
         <v>156</v>
       </c>
-      <c r="AD38" s="88" t="s">
+      <c r="AD38" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="AE38" s="89" t="s">
+      <c r="AE38" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="AF38" s="87" t="s">
+      <c r="AF38" s="85" t="s">
         <v>257</v>
       </c>
     </row>
@@ -5761,7 +5759,7 @@
       <c r="C39" s="14">
         <v>39</v>
       </c>
-      <c r="D39" s="83" t="s">
+      <c r="D39" s="81" t="s">
         <v>481</v>
       </c>
       <c r="E39" s="17" t="s">
@@ -5770,7 +5768,7 @@
       <c r="F39" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G39" s="83" t="s">
+      <c r="G39" s="81" t="s">
         <v>354</v>
       </c>
       <c r="H39" s="17">
@@ -5782,13 +5780,13 @@
       <c r="J39" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K39" s="84" t="s">
+      <c r="K39" s="82" t="s">
         <v>482</v>
       </c>
-      <c r="L39" s="81">
+      <c r="L39" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M39" s="82">
+      <c r="M39" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N39" s="68" t="s">
@@ -5800,7 +5798,7 @@
       <c r="P39" s="24">
         <v>22</v>
       </c>
-      <c r="Q39" s="85" t="s">
+      <c r="Q39" s="83" t="s">
         <v>483</v>
       </c>
       <c r="R39" s="44"/>
@@ -5815,25 +5813,25 @@
       <c r="Y39" s="24">
         <v>36</v>
       </c>
-      <c r="Z39" s="86" t="s">
+      <c r="Z39" s="84" t="s">
         <v>192</v>
       </c>
       <c r="AA39" s="17">
         <v>0.21561882598347776</v>
       </c>
-      <c r="AB39" s="84" t="s">
+      <c r="AB39" s="82" t="s">
         <v>305</v>
       </c>
-      <c r="AC39" s="83" t="s">
+      <c r="AC39" s="81" t="s">
         <v>157</v>
       </c>
-      <c r="AD39" s="88" t="s">
+      <c r="AD39" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="AE39" s="89" t="s">
+      <c r="AE39" s="87" t="s">
         <v>93</v>
       </c>
-      <c r="AF39" s="87" t="s">
+      <c r="AF39" s="85" t="s">
         <v>258</v>
       </c>
     </row>
@@ -5847,7 +5845,7 @@
       <c r="C40" s="14">
         <v>40</v>
       </c>
-      <c r="D40" s="83" t="s">
+      <c r="D40" s="81" t="s">
         <v>484</v>
       </c>
       <c r="E40" s="17" t="s">
@@ -5856,7 +5854,7 @@
       <c r="F40" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G40" s="83" t="s">
+      <c r="G40" s="81" t="s">
         <v>355</v>
       </c>
       <c r="H40" s="17">
@@ -5868,13 +5866,13 @@
       <c r="J40" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K40" s="84" t="s">
+      <c r="K40" s="82" t="s">
         <v>485</v>
       </c>
-      <c r="L40" s="81">
+      <c r="L40" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M40" s="82">
+      <c r="M40" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N40" s="68" t="s">
@@ -5886,7 +5884,7 @@
       <c r="P40" s="24">
         <v>48</v>
       </c>
-      <c r="Q40" s="85" t="s">
+      <c r="Q40" s="83" t="s">
         <v>486</v>
       </c>
       <c r="R40" s="44"/>
@@ -5901,25 +5899,25 @@
       <c r="Y40" s="24">
         <v>48</v>
       </c>
-      <c r="Z40" s="86" t="s">
+      <c r="Z40" s="84" t="s">
         <v>193</v>
       </c>
       <c r="AA40" s="17">
         <v>0.22154467361085187</v>
       </c>
-      <c r="AB40" s="105" t="s">
+      <c r="AB40" s="88" t="s">
         <v>306</v>
       </c>
-      <c r="AC40" s="83" t="s">
+      <c r="AC40" s="81" t="s">
         <v>158</v>
       </c>
-      <c r="AD40" s="88" t="s">
+      <c r="AD40" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="AE40" s="89" t="s">
+      <c r="AE40" s="87" t="s">
         <v>86</v>
       </c>
-      <c r="AF40" s="87" t="s">
+      <c r="AF40" s="85" t="s">
         <v>259</v>
       </c>
     </row>
@@ -5933,7 +5931,7 @@
       <c r="C41" s="14">
         <v>18</v>
       </c>
-      <c r="D41" s="83" t="s">
+      <c r="D41" s="81" t="s">
         <v>487</v>
       </c>
       <c r="E41" s="17" t="s">
@@ -5942,7 +5940,7 @@
       <c r="F41" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G41" s="83" t="s">
+      <c r="G41" s="81" t="s">
         <v>356</v>
       </c>
       <c r="H41" s="17">
@@ -5954,13 +5952,13 @@
       <c r="J41" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K41" s="84" t="s">
+      <c r="K41" s="82" t="s">
         <v>488</v>
       </c>
-      <c r="L41" s="81">
+      <c r="L41" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M41" s="82">
+      <c r="M41" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N41" s="68" t="s">
@@ -5972,7 +5970,7 @@
       <c r="P41" s="24">
         <v>28</v>
       </c>
-      <c r="Q41" s="85" t="s">
+      <c r="Q41" s="83" t="s">
         <v>489</v>
       </c>
       <c r="R41" s="44"/>
@@ -5987,25 +5985,25 @@
       <c r="Y41" s="24">
         <v>33</v>
       </c>
-      <c r="Z41" s="86" t="s">
+      <c r="Z41" s="84" t="s">
         <v>194</v>
       </c>
       <c r="AA41" s="17">
         <v>0.17118381997147342</v>
       </c>
-      <c r="AB41" s="84" t="s">
+      <c r="AB41" s="82" t="s">
         <v>307</v>
       </c>
-      <c r="AC41" s="83" t="s">
+      <c r="AC41" s="81" t="s">
         <v>159</v>
       </c>
-      <c r="AD41" s="88" t="s">
+      <c r="AD41" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="AE41" s="89" t="s">
+      <c r="AE41" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="AF41" s="87" t="s">
+      <c r="AF41" s="85" t="s">
         <v>260</v>
       </c>
     </row>
@@ -6019,7 +6017,7 @@
       <c r="C42" s="14">
         <v>30</v>
       </c>
-      <c r="D42" s="83" t="s">
+      <c r="D42" s="81" t="s">
         <v>490</v>
       </c>
       <c r="E42" s="17">
@@ -6028,7 +6026,7 @@
       <c r="F42" s="20">
         <v>9</v>
       </c>
-      <c r="G42" s="83" t="s">
+      <c r="G42" s="81" t="s">
         <v>357</v>
       </c>
       <c r="H42" s="17">
@@ -6040,13 +6038,13 @@
       <c r="J42" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K42" s="84" t="s">
+      <c r="K42" s="82" t="s">
         <v>491</v>
       </c>
-      <c r="L42" s="81">
+      <c r="L42" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M42" s="82">
+      <c r="M42" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N42" s="68" t="s">
@@ -6058,7 +6056,7 @@
       <c r="P42" s="24">
         <v>11</v>
       </c>
-      <c r="Q42" s="85" t="s">
+      <c r="Q42" s="83" t="s">
         <v>492</v>
       </c>
       <c r="R42" s="44"/>
@@ -6073,25 +6071,25 @@
       <c r="Y42" s="24">
         <v>6</v>
       </c>
-      <c r="Z42" s="86" t="s">
+      <c r="Z42" s="84" t="s">
         <v>195</v>
       </c>
       <c r="AA42" s="17">
         <v>0.18127382464402422</v>
       </c>
-      <c r="AB42" s="84" t="s">
+      <c r="AB42" s="82" t="s">
         <v>308</v>
       </c>
-      <c r="AC42" s="83" t="s">
+      <c r="AC42" s="81" t="s">
         <v>160</v>
       </c>
-      <c r="AD42" s="88" t="s">
+      <c r="AD42" s="86" t="s">
         <v>113</v>
       </c>
-      <c r="AE42" s="89" t="s">
+      <c r="AE42" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="AF42" s="87" t="s">
+      <c r="AF42" s="85" t="s">
         <v>261</v>
       </c>
     </row>
@@ -6105,7 +6103,7 @@
       <c r="C43" s="14">
         <v>37</v>
       </c>
-      <c r="D43" s="83" t="s">
+      <c r="D43" s="81" t="s">
         <v>493</v>
       </c>
       <c r="E43" s="17">
@@ -6114,7 +6112,7 @@
       <c r="F43" s="20">
         <v>5</v>
       </c>
-      <c r="G43" s="83" t="s">
+      <c r="G43" s="81" t="s">
         <v>358</v>
       </c>
       <c r="H43" s="17">
@@ -6126,13 +6124,13 @@
       <c r="J43" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K43" s="84" t="s">
+      <c r="K43" s="82" t="s">
         <v>494</v>
       </c>
-      <c r="L43" s="81">
+      <c r="L43" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M43" s="82">
+      <c r="M43" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N43" s="68" t="s">
@@ -6144,7 +6142,7 @@
       <c r="P43" s="24">
         <v>5</v>
       </c>
-      <c r="Q43" s="85" t="s">
+      <c r="Q43" s="83" t="s">
         <v>495</v>
       </c>
       <c r="R43" s="44"/>
@@ -6159,25 +6157,25 @@
       <c r="Y43" s="24">
         <v>2</v>
       </c>
-      <c r="Z43" s="86" t="s">
+      <c r="Z43" s="84" t="s">
         <v>196</v>
       </c>
       <c r="AA43" s="17">
         <v>0.15513360171153148</v>
       </c>
-      <c r="AB43" s="84" t="s">
+      <c r="AB43" s="82" t="s">
         <v>309</v>
       </c>
-      <c r="AC43" s="83" t="s">
+      <c r="AC43" s="81" t="s">
         <v>161</v>
       </c>
-      <c r="AD43" s="88" t="s">
+      <c r="AD43" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="AE43" s="89" t="s">
+      <c r="AE43" s="87" t="s">
         <v>79</v>
       </c>
-      <c r="AF43" s="87" t="s">
+      <c r="AF43" s="85" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6191,7 +6189,7 @@
       <c r="C44" s="14">
         <v>36</v>
       </c>
-      <c r="D44" s="83" t="s">
+      <c r="D44" s="81" t="s">
         <v>496</v>
       </c>
       <c r="E44" s="17">
@@ -6200,7 +6198,7 @@
       <c r="F44" s="20">
         <v>24</v>
       </c>
-      <c r="G44" s="83" t="s">
+      <c r="G44" s="81" t="s">
         <v>359</v>
       </c>
       <c r="H44" s="17">
@@ -6212,13 +6210,13 @@
       <c r="J44" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K44" s="84" t="s">
+      <c r="K44" s="82" t="s">
         <v>497</v>
       </c>
-      <c r="L44" s="81">
+      <c r="L44" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M44" s="82">
+      <c r="M44" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N44" s="68" t="s">
@@ -6230,7 +6228,7 @@
       <c r="P44" s="24">
         <v>23</v>
       </c>
-      <c r="Q44" s="85" t="s">
+      <c r="Q44" s="83" t="s">
         <v>498</v>
       </c>
       <c r="R44" s="44"/>
@@ -6245,25 +6243,25 @@
       <c r="Y44" s="24">
         <v>20</v>
       </c>
-      <c r="Z44" s="86" t="s">
+      <c r="Z44" s="84" t="s">
         <v>218</v>
       </c>
       <c r="AA44" s="17">
         <v>0.19657065200369842</v>
       </c>
-      <c r="AB44" s="84" t="s">
+      <c r="AB44" s="82" t="s">
         <v>310</v>
       </c>
-      <c r="AC44" s="83" t="s">
+      <c r="AC44" s="81" t="s">
         <v>162</v>
       </c>
-      <c r="AD44" s="63" t="s">
+      <c r="AD44" s="86" t="s">
         <v>85</v>
       </c>
-      <c r="AE44" s="64" t="s">
+      <c r="AE44" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="AF44" s="78" t="s">
+      <c r="AF44" s="85" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6277,7 +6275,7 @@
       <c r="C45" s="14">
         <v>12</v>
       </c>
-      <c r="D45" s="83" t="s">
+      <c r="D45" s="81" t="s">
         <v>499</v>
       </c>
       <c r="E45" s="17" t="s">
@@ -6286,7 +6284,7 @@
       <c r="F45" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G45" s="83" t="s">
+      <c r="G45" s="81" t="s">
         <v>360</v>
       </c>
       <c r="H45" s="17">
@@ -6298,13 +6296,13 @@
       <c r="J45" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K45" s="84" t="s">
+      <c r="K45" s="82" t="s">
         <v>500</v>
       </c>
-      <c r="L45" s="81">
+      <c r="L45" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M45" s="82">
+      <c r="M45" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N45" s="68" t="s">
@@ -6316,7 +6314,7 @@
       <c r="P45" s="24">
         <v>47</v>
       </c>
-      <c r="Q45" s="85" t="s">
+      <c r="Q45" s="83" t="s">
         <v>501</v>
       </c>
       <c r="R45" s="44"/>
@@ -6331,25 +6329,25 @@
       <c r="Y45" s="24">
         <v>50</v>
       </c>
-      <c r="Z45" s="86" t="s">
+      <c r="Z45" s="84" t="s">
         <v>197</v>
       </c>
       <c r="AA45" s="17">
         <v>0.20092887786830402</v>
       </c>
-      <c r="AB45" s="84" t="s">
+      <c r="AB45" s="82" t="s">
         <v>311</v>
       </c>
-      <c r="AC45" s="83" t="s">
+      <c r="AC45" s="81" t="s">
         <v>163</v>
       </c>
-      <c r="AD45" s="63" t="s">
+      <c r="AD45" s="86" t="s">
         <v>115</v>
       </c>
-      <c r="AE45" s="64" t="s">
+      <c r="AE45" s="87" t="s">
         <v>116</v>
       </c>
-      <c r="AF45" s="78" t="s">
+      <c r="AF45" s="85" t="s">
         <v>264</v>
       </c>
     </row>
@@ -6363,7 +6361,7 @@
       <c r="C46" s="14">
         <v>48</v>
       </c>
-      <c r="D46" s="14" t="s">
+      <c r="D46" s="81" t="s">
         <v>502</v>
       </c>
       <c r="E46" s="17" t="s">
@@ -6372,7 +6370,7 @@
       <c r="F46" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G46" s="14" t="s">
+      <c r="G46" s="81" t="s">
         <v>361</v>
       </c>
       <c r="H46" s="17">
@@ -6384,13 +6382,13 @@
       <c r="J46" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K46" s="19" t="s">
+      <c r="K46" s="82" t="s">
         <v>503</v>
       </c>
-      <c r="L46" s="81">
+      <c r="L46" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M46" s="82">
+      <c r="M46" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N46" s="68" t="s">
@@ -6402,7 +6400,7 @@
       <c r="P46" s="24">
         <v>20</v>
       </c>
-      <c r="Q46" s="75" t="s">
+      <c r="Q46" s="83" t="s">
         <v>504</v>
       </c>
       <c r="R46" s="44"/>
@@ -6417,25 +6415,25 @@
       <c r="Y46" s="24">
         <v>27</v>
       </c>
-      <c r="Z46" s="76" t="s">
+      <c r="Z46" s="84" t="s">
         <v>219</v>
       </c>
       <c r="AA46" s="17">
         <v>0.2190336028364763</v>
       </c>
-      <c r="AB46" s="19" t="s">
+      <c r="AB46" s="82" t="s">
         <v>312</v>
       </c>
-      <c r="AC46" s="14" t="s">
+      <c r="AC46" s="81" t="s">
         <v>164</v>
       </c>
-      <c r="AD46" s="63" t="s">
+      <c r="AD46" s="86" t="s">
         <v>117</v>
       </c>
-      <c r="AE46" s="64" t="s">
+      <c r="AE46" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="AF46" s="78" t="s">
+      <c r="AF46" s="85" t="s">
         <v>265</v>
       </c>
     </row>
@@ -6449,7 +6447,7 @@
       <c r="C47" s="14">
         <v>10</v>
       </c>
-      <c r="D47" s="14" t="s">
+      <c r="D47" s="81" t="s">
         <v>505</v>
       </c>
       <c r="E47" s="17">
@@ -6458,7 +6456,7 @@
       <c r="F47" s="20">
         <v>19</v>
       </c>
-      <c r="G47" s="14" t="s">
+      <c r="G47" s="81" t="s">
         <v>362</v>
       </c>
       <c r="H47" s="17">
@@ -6470,13 +6468,13 @@
       <c r="J47" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K47" s="19" t="s">
+      <c r="K47" s="82" t="s">
         <v>506</v>
       </c>
-      <c r="L47" s="81">
+      <c r="L47" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M47" s="82">
+      <c r="M47" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N47" s="68" t="s">
@@ -6488,7 +6486,7 @@
       <c r="P47" s="24">
         <v>44</v>
       </c>
-      <c r="Q47" s="75" t="s">
+      <c r="Q47" s="83" t="s">
         <v>507</v>
       </c>
       <c r="R47" s="44"/>
@@ -6503,25 +6501,25 @@
       <c r="Y47" s="24">
         <v>32</v>
       </c>
-      <c r="Z47" s="76" t="s">
+      <c r="Z47" s="84" t="s">
         <v>198</v>
       </c>
       <c r="AA47" s="17">
         <v>0.15209297953085757</v>
       </c>
-      <c r="AB47" s="19" t="s">
+      <c r="AB47" s="82" t="s">
         <v>313</v>
       </c>
-      <c r="AC47" s="14" t="s">
+      <c r="AC47" s="81" t="s">
         <v>165</v>
       </c>
-      <c r="AD47" s="63" t="s">
+      <c r="AD47" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="AE47" s="64" t="s">
+      <c r="AE47" s="87" t="s">
         <v>117</v>
       </c>
-      <c r="AF47" s="78" t="s">
+      <c r="AF47" s="85" t="s">
         <v>266</v>
       </c>
     </row>
@@ -6535,7 +6533,7 @@
       <c r="C48" s="14">
         <v>1</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="D48" s="81" t="s">
         <v>508</v>
       </c>
       <c r="E48" s="17">
@@ -6544,7 +6542,7 @@
       <c r="F48" s="20">
         <v>16</v>
       </c>
-      <c r="G48" s="14" t="s">
+      <c r="G48" s="81" t="s">
         <v>363</v>
       </c>
       <c r="H48" s="17">
@@ -6556,13 +6554,13 @@
       <c r="J48" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K48" s="19" t="s">
+      <c r="K48" s="82" t="s">
         <v>511</v>
       </c>
-      <c r="L48" s="81">
+      <c r="L48" s="79">
         <v>0.56200000000000006</v>
       </c>
-      <c r="M48" s="82">
+      <c r="M48" s="80">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="N48" s="68" t="s">
@@ -6574,7 +6572,7 @@
       <c r="P48" s="24">
         <v>7</v>
       </c>
-      <c r="Q48" s="75" t="s">
+      <c r="Q48" s="83" t="s">
         <v>512</v>
       </c>
       <c r="R48" s="44"/>
@@ -6589,25 +6587,25 @@
       <c r="Y48" s="24">
         <v>51</v>
       </c>
-      <c r="Z48" s="76" t="s">
+      <c r="Z48" s="84" t="s">
         <v>199</v>
       </c>
       <c r="AA48" s="17">
         <v>9.0893544929778275E-2</v>
       </c>
-      <c r="AB48" s="19" t="s">
+      <c r="AB48" s="82" t="s">
         <v>509</v>
       </c>
-      <c r="AC48" s="14" t="s">
+      <c r="AC48" s="81" t="s">
         <v>510</v>
       </c>
-      <c r="AD48" s="63" t="s">
+      <c r="AD48" s="86" t="s">
         <v>106</v>
       </c>
-      <c r="AE48" s="64" t="s">
+      <c r="AE48" s="87" t="s">
         <v>118</v>
       </c>
-      <c r="AF48" s="78" t="s">
+      <c r="AF48" s="85" t="s">
         <v>513</v>
       </c>
     </row>
@@ -6621,7 +6619,7 @@
       <c r="C49" s="14">
         <v>30</v>
       </c>
-      <c r="D49" s="14" t="s">
+      <c r="D49" s="81" t="s">
         <v>514</v>
       </c>
       <c r="E49" s="17" t="s">
@@ -6630,7 +6628,7 @@
       <c r="F49" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G49" s="14" t="s">
+      <c r="G49" s="81" t="s">
         <v>364</v>
       </c>
       <c r="H49" s="17">
@@ -6642,13 +6640,13 @@
       <c r="J49" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="K49" s="19" t="s">
+      <c r="K49" s="82" t="s">
         <v>515</v>
       </c>
-      <c r="L49" s="81">
+      <c r="L49" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M49" s="82">
+      <c r="M49" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N49" s="68" t="s">
@@ -6660,7 +6658,7 @@
       <c r="P49" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="Q49" s="75" t="s">
+      <c r="Q49" s="83" t="s">
         <v>516</v>
       </c>
       <c r="R49" s="44"/>
@@ -6675,25 +6673,25 @@
       <c r="Y49" s="24">
         <v>9</v>
       </c>
-      <c r="Z49" s="76" t="s">
+      <c r="Z49" s="84" t="s">
         <v>220</v>
       </c>
       <c r="AA49" s="17">
         <v>0.15979496413918701</v>
       </c>
-      <c r="AB49" s="19" t="s">
+      <c r="AB49" s="82" t="s">
         <v>314</v>
       </c>
-      <c r="AC49" s="14" t="s">
+      <c r="AC49" s="81" t="s">
         <v>166</v>
       </c>
-      <c r="AD49" s="63" t="s">
+      <c r="AD49" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="AE49" s="64" t="s">
+      <c r="AE49" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="AF49" s="78" t="s">
+      <c r="AF49" s="85" t="s">
         <v>267</v>
       </c>
     </row>
@@ -6707,7 +6705,7 @@
       <c r="C50" s="14">
         <v>23</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="D50" s="81" t="s">
         <v>517</v>
       </c>
       <c r="E50" s="17" t="s">
@@ -6716,7 +6714,7 @@
       <c r="F50" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G50" s="14" t="s">
+      <c r="G50" s="81" t="s">
         <v>365</v>
       </c>
       <c r="H50" s="17">
@@ -6728,13 +6726,13 @@
       <c r="J50" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K50" s="19" t="s">
+      <c r="K50" s="82" t="s">
         <v>518</v>
       </c>
-      <c r="L50" s="81">
+      <c r="L50" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M50" s="82">
+      <c r="M50" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N50" s="68" t="s">
@@ -6746,7 +6744,7 @@
       <c r="P50" s="24">
         <v>16</v>
       </c>
-      <c r="Q50" s="75" t="s">
+      <c r="Q50" s="83" t="s">
         <v>519</v>
       </c>
       <c r="R50" s="44"/>
@@ -6761,25 +6759,25 @@
       <c r="Y50" s="24">
         <v>16</v>
       </c>
-      <c r="Z50" s="76" t="s">
+      <c r="Z50" s="84" t="s">
         <v>221</v>
       </c>
       <c r="AA50" s="17">
         <v>0.16541548809560888</v>
       </c>
-      <c r="AB50" s="19" t="s">
+      <c r="AB50" s="82" t="s">
         <v>315</v>
       </c>
-      <c r="AC50" s="14" t="s">
+      <c r="AC50" s="81" t="s">
         <v>167</v>
       </c>
-      <c r="AD50" s="63" t="s">
+      <c r="AD50" s="86" t="s">
         <v>119</v>
       </c>
-      <c r="AE50" s="64" t="s">
+      <c r="AE50" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="AF50" s="78" t="s">
+      <c r="AF50" s="85" t="s">
         <v>268</v>
       </c>
     </row>
@@ -6793,7 +6791,7 @@
       <c r="C51" s="14">
         <v>19</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="D51" s="81" t="s">
         <v>520</v>
       </c>
       <c r="E51" s="17" t="s">
@@ -6802,7 +6800,7 @@
       <c r="F51" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G51" s="14" t="s">
+      <c r="G51" s="81" t="s">
         <v>366</v>
       </c>
       <c r="H51" s="17">
@@ -6814,13 +6812,13 @@
       <c r="J51" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K51" s="19" t="s">
+      <c r="K51" s="82" t="s">
         <v>521</v>
       </c>
-      <c r="L51" s="81">
+      <c r="L51" s="79">
         <v>0.63600000000000001</v>
       </c>
-      <c r="M51" s="82">
+      <c r="M51" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N51" s="68" t="s">
@@ -6832,7 +6830,7 @@
       <c r="P51" s="24">
         <v>33</v>
       </c>
-      <c r="Q51" s="75" t="s">
+      <c r="Q51" s="83" t="s">
         <v>522</v>
       </c>
       <c r="R51" s="44"/>
@@ -6847,25 +6845,25 @@
       <c r="Y51" s="24">
         <v>30</v>
       </c>
-      <c r="Z51" s="76" t="s">
+      <c r="Z51" s="84" t="s">
         <v>200</v>
       </c>
       <c r="AA51" s="17">
         <v>0.14970101143699083</v>
       </c>
-      <c r="AB51" s="19" t="s">
+      <c r="AB51" s="82" t="s">
         <v>316</v>
       </c>
-      <c r="AC51" s="14" t="s">
+      <c r="AC51" s="81" t="s">
         <v>168</v>
       </c>
-      <c r="AD51" s="63" t="s">
+      <c r="AD51" s="86" t="s">
         <v>120</v>
       </c>
-      <c r="AE51" s="64" t="s">
+      <c r="AE51" s="87" t="s">
         <v>91</v>
       </c>
-      <c r="AF51" s="78" t="s">
+      <c r="AF51" s="85" t="s">
         <v>269</v>
       </c>
     </row>
@@ -6879,7 +6877,7 @@
       <c r="C52" s="14">
         <v>50</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="81" t="s">
         <v>523</v>
       </c>
       <c r="E52" s="17">
@@ -6888,7 +6886,7 @@
       <c r="F52" s="20">
         <v>27</v>
       </c>
-      <c r="G52" s="14" t="s">
+      <c r="G52" s="81" t="s">
         <v>367</v>
       </c>
       <c r="H52" s="17">
@@ -6900,13 +6898,13 @@
       <c r="J52" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K52" s="19" t="s">
+      <c r="K52" s="82" t="s">
         <v>526</v>
       </c>
-      <c r="L52" s="81">
+      <c r="L52" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M52" s="82">
+      <c r="M52" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N52" s="68" t="s">
@@ -6918,7 +6916,7 @@
       <c r="P52" s="24">
         <v>26</v>
       </c>
-      <c r="Q52" s="75" t="s">
+      <c r="Q52" s="83" t="s">
         <v>527</v>
       </c>
       <c r="R52" s="44"/>
@@ -6933,16 +6931,16 @@
       <c r="Y52" s="24">
         <v>11</v>
       </c>
-      <c r="Z52" s="76" t="s">
+      <c r="Z52" s="84" t="s">
         <v>222</v>
       </c>
       <c r="AA52" s="17">
         <v>0.2569939381465664</v>
       </c>
-      <c r="AB52" s="19" t="s">
+      <c r="AB52" s="82" t="s">
         <v>524</v>
       </c>
-      <c r="AC52" s="14" t="s">
+      <c r="AC52" s="81" t="s">
         <v>525</v>
       </c>
       <c r="AD52" s="63" t="s">
@@ -6951,7 +6949,7 @@
       <c r="AE52" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="AF52" s="78" t="s">
+      <c r="AF52" s="76" t="s">
         <v>270</v>
       </c>
     </row>
@@ -6965,7 +6963,7 @@
       <c r="C53" s="14">
         <v>20</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="81" t="s">
         <v>528</v>
       </c>
       <c r="E53" s="17">
@@ -6974,7 +6972,7 @@
       <c r="F53" s="20">
         <v>13</v>
       </c>
-      <c r="G53" s="14" t="s">
+      <c r="G53" s="81" t="s">
         <v>368</v>
       </c>
       <c r="H53" s="17">
@@ -6986,13 +6984,13 @@
       <c r="J53" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K53" s="19" t="s">
+      <c r="K53" s="82" t="s">
         <v>529</v>
       </c>
-      <c r="L53" s="81">
+      <c r="L53" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M53" s="82">
+      <c r="M53" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N53" s="68" t="s">
@@ -7004,7 +7002,7 @@
       <c r="P53" s="24">
         <v>9</v>
       </c>
-      <c r="Q53" s="75" t="s">
+      <c r="Q53" s="83" t="s">
         <v>530</v>
       </c>
       <c r="R53" s="44"/>
@@ -7019,16 +7017,16 @@
       <c r="Y53" s="24">
         <v>41</v>
       </c>
-      <c r="Z53" s="76" t="s">
+      <c r="Z53" s="84" t="s">
         <v>201</v>
       </c>
       <c r="AA53" s="17">
         <v>0.17325688392861893</v>
       </c>
-      <c r="AB53" s="19" t="s">
+      <c r="AB53" s="82" t="s">
         <v>317</v>
       </c>
-      <c r="AC53" s="14" t="s">
+      <c r="AC53" s="81" t="s">
         <v>169</v>
       </c>
       <c r="AD53" s="63" t="s">
@@ -7037,7 +7035,7 @@
       <c r="AE53" s="64" t="s">
         <v>122</v>
       </c>
-      <c r="AF53" s="78" t="s">
+      <c r="AF53" s="76" t="s">
         <v>271</v>
       </c>
     </row>
@@ -7051,7 +7049,7 @@
       <c r="C54" s="14">
         <v>6</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="81" t="s">
         <v>531</v>
       </c>
       <c r="E54" s="17">
@@ -7060,7 +7058,7 @@
       <c r="F54" s="20">
         <v>17</v>
       </c>
-      <c r="G54" s="14" t="s">
+      <c r="G54" s="81" t="s">
         <v>369</v>
       </c>
       <c r="H54" s="17">
@@ -7072,13 +7070,13 @@
       <c r="J54" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="K54" s="19" t="s">
+      <c r="K54" s="82" t="s">
         <v>532</v>
       </c>
-      <c r="L54" s="81">
+      <c r="L54" s="79">
         <v>0.55300000000000005</v>
       </c>
-      <c r="M54" s="82">
+      <c r="M54" s="80">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N54" s="68" t="s">
@@ -7090,7 +7088,7 @@
       <c r="P54" s="24">
         <v>45</v>
       </c>
-      <c r="Q54" s="75" t="s">
+      <c r="Q54" s="83" t="s">
         <v>533</v>
       </c>
       <c r="R54" s="44"/>
@@ -7105,16 +7103,16 @@
       <c r="Y54" s="24">
         <v>49</v>
       </c>
-      <c r="Z54" s="76" t="s">
+      <c r="Z54" s="84" t="s">
         <v>202</v>
       </c>
       <c r="AA54" s="17">
         <v>0.19059345102047848</v>
       </c>
-      <c r="AB54" s="19" t="s">
+      <c r="AB54" s="82" t="s">
         <v>318</v>
       </c>
-      <c r="AC54" s="14" t="s">
+      <c r="AC54" s="81" t="s">
         <v>170</v>
       </c>
       <c r="AD54" s="63" t="s">
@@ -7123,7 +7121,7 @@
       <c r="AE54" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="AF54" s="78" t="s">
+      <c r="AF54" s="76" t="s">
         <v>272</v>
       </c>
     </row>

</xml_diff>